<commit_message>
V.8.7 -- First set of multi-var state env. experiment. REINFORCE beats all algos.
</commit_message>
<xml_diff>
--- a/analysis/Analysis_Experiments_V5_13-May-2023.xlsx
+++ b/analysis/Analysis_Experiments_V5_13-May-2023.xlsx
@@ -5,18 +5,19 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Rajesh\ResearchLab\RL_for_PdM\REINFORCE_Tool_Replace_Policy\results\13-May-2023\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Rajesh\ResearchLab\RL_for_PdM\REINFORCE_Tool_Replace_Policy\analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F65E8BA-7D4C-4F41-BACF-0402F0577CB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{042ABF74-40FC-4957-A517-88B69CDC25E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Simulated Env. Expts." sheetId="9" r:id="rId1"/>
     <sheet name="PHM Expts.-Simple State" sheetId="8" r:id="rId2"/>
     <sheet name="PHM Expts.-Multi-var State" sheetId="10" r:id="rId3"/>
     <sheet name="Notes" sheetId="6" r:id="rId4"/>
+    <sheet name="Emperical study articles" sheetId="11" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="136">
   <si>
     <t>A2C</t>
   </si>
@@ -610,6 +611,155 @@
   <si>
     <t>C-06. High noise and break-down. 1.5k episodes. 1k termination</t>
   </si>
+  <si>
+    <t>RECALL error was 1.0</t>
+  </si>
+  <si>
+    <t>Extended eps to 1200, and term to 800 - improved it drastically</t>
+  </si>
+  <si>
+    <t xml:space="preserve">force_x; force_y; force_z; vibration_x; vibration_y; vibration_z; </t>
+  </si>
+  <si>
+    <t>acoustic_emission_rms; tool_wear</t>
+  </si>
+  <si>
+    <t>Complex. Multi-variable state (8 features)</t>
+  </si>
+  <si>
+    <t>Sample Plots for REINFORCE algo. : C06 High noise and break-down chance</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">C-06. High noise and break-down. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1.5k episodes. 1k termination</t>
+    </r>
+  </si>
+  <si>
+    <t>Worse replace error. Reduced below</t>
+  </si>
+  <si>
+    <t>Worse replace error. Reduced by increasing eps. 1200 -&gt; 1500 and termination increased 800 -&gt; 1000</t>
+  </si>
+  <si>
+    <t>https://ieeexplore.ieee.org/abstract/document/9782149</t>
+  </si>
+  <si>
+    <t>An Empirical Study of Remote Sensing Pretraining</t>
+  </si>
+  <si>
+    <t>An Empirical Study of the Coolstreaming+ System</t>
+  </si>
+  <si>
+    <t>https://ieeexplore.ieee.org/abstract/document/4395123</t>
+  </si>
+  <si>
+    <t>https://ieeexplore.ieee.org/abstract/document/9054721</t>
+  </si>
+  <si>
+    <t>An Empirical Study of Conv-Tasnet</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">In this paper, we conduct an empirical study of Conv-TasNet and </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF3333FF"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>propose an enhancement</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> to the encoder/decoder that is based on a (deep) non-linear variant of it. In addition, we experiment with the larger and more diverse LibriTTS dataset and </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF3333FF"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>investigate the generalization capabilities of the studied models when trained on a much larger dataset</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">. We </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF3333FF"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>propose cross-dataset evaluation</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> that includes assessing separations from the WSJ0-2mix, LibriTTS and VCTK databases. Our results show that enhancements to the encoder/decoder can improve average SI-SNR performance by more than 1 dB. Furthermore, we offer insights into the generalization capabilities of Conv-TasNet and the potential value of improvements to the encoder/decoder.</t>
+    </r>
+  </si>
+  <si>
+    <t>A Large-Scale Empirical Study of Conficker</t>
+  </si>
+  <si>
+    <t>https://ieeexplore.ieee.org/abstract/document/6060910</t>
+  </si>
+  <si>
+    <t>Proposed enhancements</t>
+  </si>
+  <si>
+    <t>Empirical ?</t>
+  </si>
+  <si>
+    <t>"By analyzing Conficker, we intend to understand current and new trends in malware propagation, which could be very helpful in predicting future malware trends and providing insights for future malware defense.
+We measure the potential power of Conficker to estimate its effects
+This raises a question of how we can improve and complement existing reputation-based techniques to prepare for future malware defense?"</t>
+  </si>
+  <si>
+    <t>Terminate</t>
+  </si>
+  <si>
+    <t>C-06. No noise or break-down. Increase Episodes and Termination parmeters</t>
+  </si>
 </sst>
 </file>
 
@@ -619,7 +769,7 @@
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.00000"/>
   </numFmts>
-  <fonts count="32" x14ac:knownFonts="1">
+  <fonts count="38" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -858,6 +1008,55 @@
     <font>
       <b/>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3333FF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF3333FF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1286,7 +1485,7 @@
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1416,9 +1615,30 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="164" fontId="30" fillId="38" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="31" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="31" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="32" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="42" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="35" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="36" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="37" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="44">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1644,23 +1864,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>109</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>154697</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>178377</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>251762</xdr:colOff>
-      <xdr:row>125</xdr:row>
-      <xdr:rowOff>72390</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>1424563</xdr:colOff>
+      <xdr:row>82</xdr:row>
+      <xdr:rowOff>86663</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
+        <xdr:cNvPr id="8" name="Picture 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7327808C-B630-4C30-879F-74EC0ED4B6B5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{861EF22A-DC29-5D71-5D32-4207D9ADEA54}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1682,8 +1902,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="609600" y="12144375"/>
-          <a:ext cx="7772814" cy="3108960"/>
+          <a:off x="6358371" y="17513877"/>
+          <a:ext cx="5485714" cy="2194286"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1694,23 +1914,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>126</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>135392</xdr:colOff>
+      <xdr:row>82</xdr:row>
+      <xdr:rowOff>103204</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>251762</xdr:colOff>
-      <xdr:row>142</xdr:row>
-      <xdr:rowOff>72390</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>1405258</xdr:colOff>
+      <xdr:row>94</xdr:row>
+      <xdr:rowOff>11490</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2">
+        <xdr:cNvPr id="10" name="Picture 9">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EA67AC1B-8822-4D1E-82DC-0386BC28EFE1}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A2A8BE76-793B-AA46-14C5-87BF54F064C3}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1732,8 +1952,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="609600" y="15382875"/>
-          <a:ext cx="7772814" cy="3108960"/>
+          <a:off x="6339066" y="19724704"/>
+          <a:ext cx="5485714" cy="2194286"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1744,23 +1964,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>144</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>504354</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>188298</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>251762</xdr:colOff>
-      <xdr:row>160</xdr:row>
-      <xdr:rowOff>72390</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>415872</xdr:colOff>
+      <xdr:row>82</xdr:row>
+      <xdr:rowOff>96584</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3">
+        <xdr:cNvPr id="12" name="Picture 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{88CDCCFD-FF29-47EA-A597-ED317E88E86B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{39B790CC-F104-AEFA-4893-C2872C31E42B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1782,8 +2002,58 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="609600" y="18811875"/>
-          <a:ext cx="7772814" cy="3108960"/>
+          <a:off x="504354" y="17523798"/>
+          <a:ext cx="5485714" cy="2194286"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>598560</xdr:colOff>
+      <xdr:row>82</xdr:row>
+      <xdr:rowOff>80860</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>510078</xdr:colOff>
+      <xdr:row>93</xdr:row>
+      <xdr:rowOff>179646</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="14" name="Picture 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4C967600-878A-A0E7-63B6-0E19BE6334C6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="598560" y="19702360"/>
+          <a:ext cx="5485714" cy="2194286"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1796,161 +2066,6 @@
 </file>
 
 <file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>109</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>251762</xdr:colOff>
-      <xdr:row>125</xdr:row>
-      <xdr:rowOff>72390</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4913BE03-FA04-4DE8-9944-D137731EE634}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="609600" y="24298275"/>
-          <a:ext cx="7719362" cy="3120390"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>126</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>251762</xdr:colOff>
-      <xdr:row>142</xdr:row>
-      <xdr:rowOff>72390</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F7DB8D8A-B483-41B0-9A2E-8AD76AA32FE9}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="609600" y="27536775"/>
-          <a:ext cx="7719362" cy="3120390"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>144</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>251762</xdr:colOff>
-      <xdr:row>160</xdr:row>
-      <xdr:rowOff>72390</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A4C78614-0D24-45CF-A39E-805ED0B33EE7}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="609600" y="30965775"/>
-          <a:ext cx="7719362" cy="3120390"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
@@ -2773,7 +2888,7 @@
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A5" sqref="A5:XFD22"/>
+      <selection pane="bottomLeft" activeCell="N26" sqref="N26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3671,11 +3786,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D002316C-426C-49E1-8B50-2FDC1BA0BFFE}">
-  <dimension ref="A2:W125"/>
+  <dimension ref="A2:W87"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G66" sqref="G66"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="4" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F53" sqref="F53:M53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3970,6 +4085,12 @@
       <c r="T9" s="53"/>
     </row>
     <row r="10" spans="1:20" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C10" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="D10" s="48">
+        <v>800</v>
+      </c>
       <c r="P10" s="3" t="s">
         <v>19</v>
       </c>
@@ -4167,6 +4288,12 @@
       </c>
     </row>
     <row r="16" spans="1:20" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C16" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="D16" s="48">
+        <v>800</v>
+      </c>
       <c r="E16" s="35"/>
       <c r="J16" s="7"/>
       <c r="L16" s="7"/>
@@ -4376,6 +4503,12 @@
       <c r="R21"/>
     </row>
     <row r="22" spans="1:23" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C22" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="D22" s="48">
+        <v>800</v>
+      </c>
       <c r="J22" s="7"/>
       <c r="L22" s="7"/>
       <c r="M22" s="7"/>
@@ -4600,6 +4733,12 @@
       <c r="R28"/>
     </row>
     <row r="29" spans="1:23" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C29" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="D29" s="48">
+        <v>800</v>
+      </c>
       <c r="Q29"/>
       <c r="R29"/>
     </row>
@@ -4792,6 +4931,12 @@
       <c r="N34" s="1"/>
     </row>
     <row r="35" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C35" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="D35" s="48">
+        <v>800</v>
+      </c>
       <c r="E35" s="35"/>
       <c r="J35" s="7"/>
       <c r="L35" s="7"/>
@@ -4963,6 +5108,12 @@
       <c r="N40" s="1"/>
     </row>
     <row r="41" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C41" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="D41" s="48">
+        <v>800</v>
+      </c>
       <c r="N41" s="1"/>
     </row>
     <row r="42" spans="1:14" ht="30" x14ac:dyDescent="0.25">
@@ -5174,7 +5325,14 @@
       </c>
       <c r="N47" s="1"/>
     </row>
-    <row r="48" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="48" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C48" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="D48" s="48">
+        <v>800</v>
+      </c>
+    </row>
     <row r="49" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B49" s="15" t="s">
         <v>89</v>
@@ -5340,6 +5498,12 @@
       <c r="N53" s="1"/>
     </row>
     <row r="54" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C54" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="D54" s="48">
+        <v>800</v>
+      </c>
       <c r="E54" s="35"/>
       <c r="J54" s="7"/>
       <c r="L54" s="7"/>
@@ -5508,316 +5672,256 @@
       <c r="M59" s="9">
         <v>0.34</v>
       </c>
-      <c r="N59" s="1"/>
+      <c r="N59" s="42" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="60" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C60" s="6"/>
-      <c r="N60" s="1"/>
+      <c r="C60" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D60" s="48">
+        <v>800</v>
+      </c>
+      <c r="E60" s="35"/>
+      <c r="F60" s="9"/>
+      <c r="G60" s="9"/>
+      <c r="H60" s="9"/>
+      <c r="I60" s="9"/>
+      <c r="J60" s="9"/>
+      <c r="K60" s="9"/>
+      <c r="L60" s="56"/>
+      <c r="M60" s="9"/>
+      <c r="N60" s="42"/>
     </row>
     <row r="61" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B61" s="15" t="s">
-        <v>112</v>
-      </c>
-      <c r="C61" s="16"/>
-      <c r="D61" s="16"/>
-      <c r="E61" s="46"/>
-      <c r="F61" s="17"/>
-      <c r="G61" s="17"/>
-      <c r="H61" s="17"/>
-      <c r="I61" s="17"/>
-      <c r="J61" s="17"/>
-      <c r="K61" s="17"/>
-      <c r="L61" s="17"/>
-      <c r="M61" s="17"/>
-      <c r="N61" s="17"/>
+      <c r="C61" s="6"/>
+      <c r="N61" s="1"/>
     </row>
     <row r="62" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B62" s="3" t="s">
+      <c r="B62" s="15" t="s">
+        <v>119</v>
+      </c>
+      <c r="C62" s="16"/>
+      <c r="D62" s="16"/>
+      <c r="E62" s="46"/>
+      <c r="F62" s="17"/>
+      <c r="G62" s="17"/>
+      <c r="H62" s="17"/>
+      <c r="I62" s="17"/>
+      <c r="J62" s="17"/>
+      <c r="K62" s="17"/>
+      <c r="L62" s="17"/>
+      <c r="M62" s="17"/>
+      <c r="N62" s="17"/>
+    </row>
+    <row r="63" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B63" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C62" s="2" t="s">
+      <c r="C63" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="D62" s="44">
+      <c r="D63" s="44">
         <v>0.13</v>
       </c>
-      <c r="E62" s="39" t="s">
+      <c r="E63" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="F62" s="57"/>
-      <c r="G62" s="57"/>
-      <c r="H62" s="57"/>
-      <c r="I62" s="57"/>
-      <c r="J62" s="57"/>
-      <c r="K62" s="57"/>
-      <c r="L62" s="57"/>
-      <c r="M62" s="57"/>
-    </row>
-    <row r="63" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C63" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="D63" s="55" t="s">
-        <v>105</v>
-      </c>
-      <c r="E63" s="39" t="s">
+      <c r="F63" s="57">
+        <v>0.39387499999999998</v>
+      </c>
+      <c r="G63" s="57">
+        <v>0.625</v>
+      </c>
+      <c r="H63" s="57">
+        <v>0.4249</v>
+      </c>
+      <c r="I63" s="57">
+        <v>0.45360899999999998</v>
+      </c>
+      <c r="J63" s="57">
+        <v>0.48224499999999998</v>
+      </c>
+      <c r="K63" s="57">
+        <v>0</v>
+      </c>
+      <c r="L63" s="57">
         <v>1</v>
       </c>
-      <c r="F63" s="57"/>
-      <c r="G63" s="57"/>
-      <c r="H63" s="57"/>
-      <c r="I63" s="57"/>
-      <c r="J63" s="57"/>
-      <c r="K63" s="57"/>
-      <c r="L63" s="57"/>
-      <c r="M63" s="57"/>
+      <c r="M63" s="57">
+        <v>0.375</v>
+      </c>
     </row>
     <row r="64" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C64" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D64" s="55" t="s">
+        <v>105</v>
+      </c>
+      <c r="E64" s="39" t="s">
+        <v>1</v>
+      </c>
+      <c r="F64" s="57">
+        <v>0.48565000000000003</v>
+      </c>
+      <c r="G64" s="57">
+        <v>0.6</v>
+      </c>
+      <c r="H64" s="57">
+        <v>0.44285200000000002</v>
+      </c>
+      <c r="I64" s="57">
+        <v>0.45757399999999998</v>
+      </c>
+      <c r="J64" s="57">
+        <v>0.47864400000000001</v>
+      </c>
+      <c r="K64" s="57">
+        <v>4.2125000000000003E-2</v>
+      </c>
+      <c r="L64" s="57">
+        <v>0.97614000000000001</v>
+      </c>
+      <c r="M64" s="57">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="65" spans="2:22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C65" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="D64" s="49">
+      <c r="D65" s="49">
         <v>0.1</v>
       </c>
-      <c r="E64" s="39" t="s">
+      <c r="E65" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="F64" s="57"/>
-      <c r="G64" s="57"/>
-      <c r="H64" s="57"/>
-      <c r="I64" s="57"/>
-      <c r="J64" s="57"/>
-      <c r="K64" s="57"/>
-      <c r="L64" s="57"/>
-      <c r="M64" s="57"/>
-    </row>
-    <row r="65" spans="3:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C65" s="2" t="s">
+      <c r="F65" s="57">
+        <v>0.53642900000000004</v>
+      </c>
+      <c r="G65" s="57">
+        <v>0.495</v>
+      </c>
+      <c r="H65" s="57">
+        <v>0.51601399999999997</v>
+      </c>
+      <c r="I65" s="57">
+        <v>0.50471999999999995</v>
+      </c>
+      <c r="J65" s="57">
+        <v>0.49790699999999999</v>
+      </c>
+      <c r="K65" s="57">
+        <v>0.53065600000000002</v>
+      </c>
+      <c r="L65" s="57">
+        <v>0.45722499999999999</v>
+      </c>
+      <c r="M65" s="57">
+        <v>0.505</v>
+      </c>
+    </row>
+    <row r="66" spans="2:22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C66" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="D65" s="48">
+      <c r="D66" s="66">
         <v>1500</v>
       </c>
-      <c r="E65" s="35" t="s">
+      <c r="E66" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="F65" s="58"/>
-      <c r="G65" s="58"/>
-      <c r="H65" s="58"/>
-      <c r="I65" s="58"/>
-      <c r="J65" s="58"/>
-      <c r="K65" s="58"/>
-      <c r="L65" s="58"/>
-      <c r="M65" s="58"/>
-    </row>
-    <row r="66" spans="3:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C66" s="59" t="s">
+      <c r="F66" s="9">
+        <v>0.84449700000000005</v>
+      </c>
+      <c r="G66" s="9">
+        <v>0.79500000000000004</v>
+      </c>
+      <c r="H66" s="9">
+        <v>0.81926900000000002</v>
+      </c>
+      <c r="I66" s="9">
+        <v>0.80498899999999995</v>
+      </c>
+      <c r="J66" s="9">
+        <v>0.79644099999999995</v>
+      </c>
+      <c r="K66" s="9">
+        <v>0.303203</v>
+      </c>
+      <c r="L66" s="9">
+        <v>5.3332999999999998E-2</v>
+      </c>
+      <c r="M66" s="9">
+        <v>0.20499999999999999</v>
+      </c>
+      <c r="N66" s="42" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="67" spans="2:22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C67" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="D66" s="48">
+      <c r="D67" s="66">
         <v>1000</v>
       </c>
-      <c r="N66" s="1"/>
-    </row>
-    <row r="67" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C67" s="6"/>
       <c r="N67" s="1"/>
     </row>
-    <row r="68" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C68" s="6"/>
       <c r="N68" s="1"/>
     </row>
-    <row r="69" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C69" s="6"/>
+    <row r="69" spans="2:22" x14ac:dyDescent="0.25">
       <c r="N69" s="1"/>
     </row>
-    <row r="70" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C70" s="6"/>
-      <c r="N70" s="1"/>
-    </row>
-    <row r="71" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C71" s="6"/>
-      <c r="N71" s="1"/>
-    </row>
-    <row r="72" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C72" s="6"/>
-      <c r="N72" s="1"/>
-    </row>
-    <row r="73" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C73" s="6"/>
-      <c r="N73" s="1"/>
-    </row>
-    <row r="74" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C74" s="6"/>
-      <c r="N74" s="1"/>
-    </row>
-    <row r="75" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C75" s="6"/>
-      <c r="N75" s="1"/>
-    </row>
-    <row r="76" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C76" s="6"/>
-      <c r="N76" s="1"/>
-    </row>
-    <row r="77" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C77" s="6"/>
-      <c r="N77" s="1"/>
-    </row>
-    <row r="78" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C78" s="6"/>
-      <c r="N78" s="1"/>
-    </row>
-    <row r="79" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C79" s="6"/>
-      <c r="N79" s="1"/>
-    </row>
-    <row r="80" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C80" s="6"/>
-      <c r="N80" s="1"/>
-    </row>
-    <row r="81" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C81" s="6"/>
-      <c r="N81" s="1"/>
-    </row>
-    <row r="82" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C82" s="6"/>
-      <c r="N82" s="1"/>
-    </row>
-    <row r="83" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C83" s="6"/>
-      <c r="N83" s="1"/>
-    </row>
-    <row r="84" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C84" s="6"/>
-      <c r="N84" s="1"/>
-    </row>
-    <row r="85" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C85" s="6"/>
-      <c r="N85" s="1"/>
-    </row>
-    <row r="86" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C86" s="6"/>
-      <c r="N86" s="1"/>
-    </row>
-    <row r="87" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C87" s="6"/>
-      <c r="N87" s="1"/>
-    </row>
-    <row r="88" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C88" s="6"/>
-      <c r="N88" s="1"/>
-    </row>
-    <row r="89" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C89" s="6"/>
-      <c r="N89" s="1"/>
-    </row>
-    <row r="90" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C90" s="6"/>
-      <c r="N90" s="1"/>
-    </row>
-    <row r="91" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C91" s="6"/>
-      <c r="N91" s="1"/>
-    </row>
-    <row r="92" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C92" s="6"/>
-      <c r="N92" s="1"/>
-    </row>
-    <row r="93" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C93" s="6"/>
-      <c r="N93" s="1"/>
-    </row>
-    <row r="94" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C94" s="6"/>
-      <c r="N94" s="1"/>
-    </row>
-    <row r="95" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C95" s="6"/>
-      <c r="N95" s="1"/>
-    </row>
-    <row r="96" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C96" s="6"/>
-      <c r="N96" s="1"/>
-    </row>
-    <row r="97" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="C97" s="6"/>
-      <c r="N97" s="1"/>
-    </row>
-    <row r="98" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="C98" s="6"/>
-      <c r="N98" s="1"/>
-    </row>
-    <row r="99" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="C99" s="6"/>
-      <c r="N99" s="1"/>
-    </row>
-    <row r="100" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="C100" s="6"/>
-      <c r="N100" s="1"/>
-    </row>
-    <row r="101" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="C101" s="6"/>
-      <c r="N101" s="1"/>
-    </row>
-    <row r="102" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="C102" s="6"/>
-      <c r="N102" s="1"/>
-    </row>
-    <row r="103" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="C103" s="6"/>
-      <c r="N103" s="1"/>
-    </row>
-    <row r="104" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="N104" s="1"/>
-    </row>
-    <row r="105" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="N105" s="1"/>
-    </row>
-    <row r="106" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="E106" s="35"/>
-      <c r="N106" s="1"/>
-    </row>
-    <row r="107" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="N107" s="1"/>
-    </row>
-    <row r="108" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B108" s="22" t="s">
-        <v>40</v>
-      </c>
-      <c r="C108" s="23"/>
-      <c r="D108" s="23"/>
-      <c r="E108" s="47"/>
-      <c r="F108" s="24"/>
-      <c r="G108" s="24"/>
-      <c r="H108" s="24"/>
-      <c r="I108" s="24"/>
-      <c r="J108" s="24"/>
-      <c r="K108" s="24"/>
-      <c r="L108" s="25"/>
-      <c r="M108" s="43"/>
-    </row>
-    <row r="109" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B109"/>
-      <c r="C109"/>
-      <c r="D109"/>
-      <c r="E109" s="3"/>
-      <c r="F109"/>
-      <c r="G109"/>
-      <c r="H109"/>
-      <c r="I109"/>
-      <c r="J109"/>
-      <c r="K109"/>
-      <c r="L109"/>
-      <c r="M109"/>
-    </row>
-    <row r="124" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P124" s="3"/>
-      <c r="Q124"/>
-      <c r="R124"/>
-    </row>
-    <row r="125" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="Q125"/>
-      <c r="R125"/>
+    <row r="70" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B70" s="22" t="s">
+        <v>118</v>
+      </c>
+      <c r="C70" s="23"/>
+      <c r="D70" s="23"/>
+      <c r="E70" s="47"/>
+      <c r="F70" s="24"/>
+      <c r="G70" s="24"/>
+      <c r="H70" s="24"/>
+      <c r="I70" s="24"/>
+      <c r="J70" s="24"/>
+      <c r="K70" s="24"/>
+      <c r="L70" s="25"/>
+      <c r="M70" s="25"/>
+      <c r="N70" s="25"/>
+      <c r="O70" s="25"/>
+      <c r="P70" s="25"/>
+      <c r="S70" s="3"/>
+      <c r="T70" s="3"/>
+      <c r="U70" s="3"/>
+      <c r="V70" s="3"/>
+    </row>
+    <row r="71" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B71"/>
+      <c r="C71"/>
+      <c r="D71"/>
+      <c r="E71" s="3"/>
+      <c r="F71"/>
+      <c r="G71"/>
+      <c r="H71"/>
+      <c r="I71"/>
+      <c r="J71"/>
+      <c r="K71"/>
+      <c r="L71"/>
+      <c r="M71"/>
+    </row>
+    <row r="86" spans="16:18" x14ac:dyDescent="0.25">
+      <c r="P86" s="3"/>
+      <c r="Q86"/>
+      <c r="R86"/>
+    </row>
+    <row r="87" spans="16:18" x14ac:dyDescent="0.25">
+      <c r="Q87"/>
+      <c r="R87"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5828,17 +5932,17 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE699FEF-4516-4E3F-8EE7-4192FF715912}">
-  <dimension ref="A2:W125"/>
+  <dimension ref="A2:W137"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F25" sqref="F25:N28"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="4" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F54" sqref="F54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="7.7109375" style="3" customWidth="1"/>
-    <col min="3" max="3" width="12.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.140625" style="2" customWidth="1"/>
     <col min="5" max="5" width="15.28515625" style="39" customWidth="1"/>
     <col min="6" max="13" width="9.42578125" style="1" customWidth="1"/>
@@ -6037,12 +6141,10 @@
       <c r="M8" s="57"/>
     </row>
     <row r="9" spans="1:20" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D9" s="48">
-        <v>1200</v>
-      </c>
+      <c r="D9" s="63"/>
       <c r="E9" s="35" t="s">
         <v>3</v>
       </c>
@@ -6063,6 +6165,10 @@
       <c r="T9" s="53"/>
     </row>
     <row r="10" spans="1:20" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C10" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="D10" s="63"/>
       <c r="P10" s="3" t="s">
         <v>19</v>
       </c>
@@ -6170,12 +6276,10 @@
       <c r="T14" s="53"/>
     </row>
     <row r="15" spans="1:20" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C15" s="2" t="s">
+      <c r="C15" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D15" s="48">
-        <v>1200</v>
-      </c>
+      <c r="D15" s="63"/>
       <c r="E15" s="35" t="s">
         <v>3</v>
       </c>
@@ -6192,10 +6296,14 @@
         <v>95</v>
       </c>
       <c r="Q15" s="3" t="s">
-        <v>96</v>
+        <v>117</v>
       </c>
     </row>
     <row r="16" spans="1:20" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C16" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="D16" s="63"/>
       <c r="E16" s="35"/>
       <c r="J16" s="7"/>
       <c r="L16" s="7"/>
@@ -6205,7 +6313,7 @@
         <v>100</v>
       </c>
       <c r="Q16" s="3" t="s">
-        <v>101</v>
+        <v>115</v>
       </c>
     </row>
     <row r="17" spans="1:23" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -6224,11 +6332,8 @@
       <c r="L17" s="17"/>
       <c r="M17" s="17"/>
       <c r="N17" s="17"/>
-      <c r="P17" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q17" s="3">
-        <v>1200</v>
+      <c r="Q17" s="3" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="18" spans="1:23" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -6254,10 +6359,10 @@
       <c r="M18" s="57"/>
       <c r="N18" s="1"/>
       <c r="P18" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="Q18" s="3">
-        <v>800</v>
+        <v>51</v>
+      </c>
+      <c r="Q18" s="62">
+        <v>1500</v>
       </c>
     </row>
     <row r="19" spans="1:23" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -6280,10 +6385,10 @@
       <c r="M19" s="57"/>
       <c r="N19" s="1"/>
       <c r="P19" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="Q19" s="3" t="s">
-        <v>99</v>
+        <v>97</v>
+      </c>
+      <c r="Q19" s="62">
+        <v>1000</v>
       </c>
     </row>
     <row r="20" spans="1:23" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -6306,20 +6411,17 @@
       <c r="M20" s="57"/>
       <c r="N20" s="1"/>
       <c r="P20" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="Q20" s="3">
-        <v>40</v>
-      </c>
-      <c r="R20"/>
+        <v>56</v>
+      </c>
+      <c r="Q20" s="3" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="21" spans="1:23" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C21" s="2" t="s">
+      <c r="C21" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D21" s="48">
-        <v>1200</v>
-      </c>
+      <c r="D21" s="63"/>
       <c r="E21" s="35" t="s">
         <v>3</v>
       </c>
@@ -6333,23 +6435,27 @@
       <c r="M21" s="58"/>
       <c r="N21" s="1"/>
       <c r="P21" s="3" t="s">
-        <v>98</v>
+        <v>58</v>
       </c>
       <c r="Q21" s="3">
-        <v>5</v>
+        <v>40</v>
       </c>
       <c r="R21"/>
     </row>
     <row r="22" spans="1:23" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C22" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="D22" s="63"/>
       <c r="J22" s="7"/>
       <c r="L22" s="7"/>
       <c r="M22" s="7"/>
       <c r="N22" s="1"/>
       <c r="P22" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="Q22" s="3" t="s">
-        <v>111</v>
+        <v>98</v>
+      </c>
+      <c r="Q22" s="3">
+        <v>5</v>
       </c>
       <c r="R22"/>
     </row>
@@ -6392,8 +6498,13 @@
       <c r="N23" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="Q23"/>
-      <c r="R23"/>
+      <c r="P23" s="61" t="s">
+        <v>110</v>
+      </c>
+      <c r="Q23" s="61" t="s">
+        <v>111</v>
+      </c>
+      <c r="R23" s="60"/>
     </row>
     <row r="24" spans="1:23" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="15" t="s">
@@ -6483,9 +6594,7 @@
       <c r="C28" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="D28" s="48">
-        <v>1200</v>
-      </c>
+      <c r="D28" s="48"/>
       <c r="E28" s="35" t="s">
         <v>3</v>
       </c>
@@ -6612,9 +6721,7 @@
       <c r="C34" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="D34" s="48">
-        <v>1200</v>
-      </c>
+      <c r="D34" s="48"/>
       <c r="E34" s="35" t="s">
         <v>3</v>
       </c>
@@ -6719,9 +6826,7 @@
       <c r="C40" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="D40" s="48">
-        <v>1200</v>
-      </c>
+      <c r="D40" s="48"/>
       <c r="E40" s="35" t="s">
         <v>3</v>
       </c>
@@ -6812,14 +6917,30 @@
       <c r="E44" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="F44" s="57"/>
-      <c r="G44" s="57"/>
-      <c r="H44" s="57"/>
-      <c r="I44" s="57"/>
-      <c r="J44" s="57"/>
-      <c r="K44" s="57"/>
-      <c r="L44" s="57"/>
-      <c r="M44" s="57"/>
+      <c r="F44" s="57">
+        <v>0.54417899999999997</v>
+      </c>
+      <c r="G44" s="67">
+        <v>0.53</v>
+      </c>
+      <c r="H44" s="67">
+        <v>0.53493800000000002</v>
+      </c>
+      <c r="I44" s="67">
+        <v>0.53006200000000003</v>
+      </c>
+      <c r="J44" s="57">
+        <v>0.52746000000000004</v>
+      </c>
+      <c r="K44" s="67">
+        <v>0.36816199999999999</v>
+      </c>
+      <c r="L44" s="57">
+        <v>0.62563199999999997</v>
+      </c>
+      <c r="M44" s="67">
+        <v>0.47</v>
+      </c>
       <c r="N44" s="1"/>
     </row>
     <row r="45" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -6833,14 +6954,30 @@
       <c r="E45" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="F45" s="57"/>
-      <c r="G45" s="57"/>
-      <c r="H45" s="57"/>
-      <c r="I45" s="57"/>
-      <c r="J45" s="57"/>
-      <c r="K45" s="57"/>
-      <c r="L45" s="57"/>
-      <c r="M45" s="57"/>
+      <c r="F45" s="57">
+        <v>0.46665400000000001</v>
+      </c>
+      <c r="G45" s="57">
+        <v>0.34</v>
+      </c>
+      <c r="H45" s="57">
+        <v>0.24832299999999999</v>
+      </c>
+      <c r="I45" s="57">
+        <v>0.223049</v>
+      </c>
+      <c r="J45" s="57">
+        <v>0.22284200000000001</v>
+      </c>
+      <c r="K45" s="57">
+        <v>0.95034099999999999</v>
+      </c>
+      <c r="L45" s="57">
+        <v>6.0233000000000002E-2</v>
+      </c>
+      <c r="M45" s="57">
+        <v>0.66</v>
+      </c>
       <c r="N45" s="1"/>
     </row>
     <row r="46" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -6853,40 +6990,79 @@
       <c r="E46" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="F46" s="57"/>
-      <c r="G46" s="57"/>
-      <c r="H46" s="57"/>
-      <c r="I46" s="57"/>
-      <c r="J46" s="57"/>
-      <c r="K46" s="57"/>
-      <c r="L46" s="57"/>
-      <c r="M46" s="57"/>
+      <c r="F46" s="57">
+        <v>0.53305899999999995</v>
+      </c>
+      <c r="G46" s="57">
+        <v>0.51500000000000001</v>
+      </c>
+      <c r="H46" s="57">
+        <v>0.52414499999999997</v>
+      </c>
+      <c r="I46" s="57">
+        <v>0.51906799999999997</v>
+      </c>
+      <c r="J46" s="67">
+        <v>0.51599899999999999</v>
+      </c>
+      <c r="K46" s="57">
+        <v>0.41410999999999998</v>
+      </c>
+      <c r="L46" s="57">
+        <v>0.56725400000000004</v>
+      </c>
+      <c r="M46" s="57">
+        <v>0.48499999999999999</v>
+      </c>
       <c r="N46" s="1"/>
     </row>
     <row r="47" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C47" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="D47" s="48">
+      <c r="D47" s="63">
         <v>1200</v>
       </c>
       <c r="E47" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="F47" s="58"/>
-      <c r="G47" s="58"/>
-      <c r="H47" s="58"/>
-      <c r="I47" s="58"/>
-      <c r="J47" s="58"/>
-      <c r="K47" s="58"/>
-      <c r="L47" s="58"/>
-      <c r="M47" s="58"/>
+      <c r="F47" s="9">
+        <v>0.79397600000000002</v>
+      </c>
+      <c r="G47" s="57">
+        <v>0.495</v>
+      </c>
+      <c r="H47" s="68">
+        <v>0.51964100000000002</v>
+      </c>
+      <c r="I47" s="57">
+        <v>0.45324900000000001</v>
+      </c>
+      <c r="J47" s="57">
+        <v>0.42981900000000001</v>
+      </c>
+      <c r="K47" s="57">
+        <v>0.79665699999999995</v>
+      </c>
+      <c r="L47" s="9">
+        <v>0</v>
+      </c>
+      <c r="M47" s="57">
+        <v>0.505</v>
+      </c>
       <c r="N47" s="1"/>
     </row>
-    <row r="48" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="48" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C48" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D48" s="63">
+        <v>800</v>
+      </c>
+    </row>
     <row r="49" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B49" s="15" t="s">
-        <v>89</v>
+        <v>135</v>
       </c>
       <c r="C49" s="16"/>
       <c r="D49" s="16"/>
@@ -6914,34 +7090,67 @@
       <c r="E50" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="F50" s="57"/>
-      <c r="G50" s="57"/>
-      <c r="H50" s="57"/>
-      <c r="I50" s="57"/>
-      <c r="J50" s="57"/>
-      <c r="K50" s="57"/>
-      <c r="L50" s="57"/>
-      <c r="M50" s="57"/>
+      <c r="F50" s="57">
+        <v>0.55370799999999998</v>
+      </c>
+      <c r="G50" s="57">
+        <v>0.435</v>
+      </c>
+      <c r="H50" s="57">
+        <v>0.403055</v>
+      </c>
+      <c r="I50" s="57">
+        <v>0.368703</v>
+      </c>
+      <c r="J50" s="57">
+        <v>0.36066399999999998</v>
+      </c>
+      <c r="K50" s="57">
+        <v>0.86304099999999995</v>
+      </c>
+      <c r="L50" s="67">
+        <v>0.136935</v>
+      </c>
+      <c r="M50" s="57">
+        <v>0.56499999999999995</v>
+      </c>
       <c r="N50" s="1"/>
     </row>
     <row r="51" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B51" s="2"/>
       <c r="C51" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="D51" s="55" t="s">
-        <v>104</v>
+      <c r="D51" s="54" t="s">
+        <v>103</v>
       </c>
       <c r="E51" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="F51" s="57"/>
-      <c r="G51" s="57"/>
-      <c r="H51" s="57"/>
-      <c r="I51" s="57"/>
-      <c r="J51" s="57"/>
-      <c r="K51" s="57"/>
-      <c r="L51" s="57"/>
-      <c r="M51" s="57"/>
+      <c r="F51" s="57">
+        <v>0.62873199999999996</v>
+      </c>
+      <c r="G51" s="57">
+        <v>0.64</v>
+      </c>
+      <c r="H51" s="57">
+        <v>0.50267099999999998</v>
+      </c>
+      <c r="I51" s="57">
+        <v>0.50503200000000004</v>
+      </c>
+      <c r="J51" s="57">
+        <v>0.52159199999999994</v>
+      </c>
+      <c r="K51" s="57">
+        <v>7.6920000000000001E-3</v>
+      </c>
+      <c r="L51" s="57">
+        <v>0.94906000000000001</v>
+      </c>
+      <c r="M51" s="57">
+        <v>0.36</v>
+      </c>
       <c r="N51" s="1"/>
     </row>
     <row r="52" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -6949,155 +7158,108 @@
         <v>77</v>
       </c>
       <c r="D52" s="49">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="E52" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="F52" s="57"/>
-      <c r="G52" s="57"/>
-      <c r="H52" s="57"/>
-      <c r="I52" s="57"/>
-      <c r="J52" s="57"/>
-      <c r="K52" s="57"/>
-      <c r="L52" s="57"/>
-      <c r="M52" s="57"/>
+      <c r="F52" s="57">
+        <v>0.51003699999999996</v>
+      </c>
+      <c r="G52" s="57">
+        <v>0.505</v>
+      </c>
+      <c r="H52" s="57">
+        <v>0.50768899999999995</v>
+      </c>
+      <c r="I52" s="57">
+        <v>0.50630900000000001</v>
+      </c>
+      <c r="J52" s="57">
+        <v>0.50545200000000001</v>
+      </c>
+      <c r="K52" s="57">
+        <v>0.49773899999999999</v>
+      </c>
+      <c r="L52" s="57">
+        <v>0.49839899999999998</v>
+      </c>
+      <c r="M52" s="57">
+        <v>0.495</v>
+      </c>
       <c r="N52" s="1"/>
     </row>
     <row r="53" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C53" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="D53" s="48">
-        <v>1200</v>
+      <c r="D53" s="63">
+        <v>1500</v>
       </c>
       <c r="E53" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="F53" s="58"/>
-      <c r="G53" s="58"/>
-      <c r="H53" s="58"/>
-      <c r="I53" s="58"/>
-      <c r="J53" s="58"/>
-      <c r="K53" s="58"/>
-      <c r="L53" s="58"/>
-      <c r="M53" s="58"/>
+      <c r="F53" s="9">
+        <v>0.85310600000000003</v>
+      </c>
+      <c r="G53" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="H53" s="9">
+        <v>0.80689699999999998</v>
+      </c>
+      <c r="I53" s="9">
+        <v>0.78798400000000002</v>
+      </c>
+      <c r="J53" s="9">
+        <v>0.78028200000000003</v>
+      </c>
+      <c r="K53" s="9">
+        <v>0</v>
+      </c>
+      <c r="L53" s="57">
+        <v>0.49335699999999999</v>
+      </c>
+      <c r="M53" s="9">
+        <v>0.2</v>
+      </c>
       <c r="N53" s="1"/>
     </row>
     <row r="54" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E54" s="35"/>
-      <c r="J54" s="7"/>
-      <c r="L54" s="7"/>
-      <c r="M54" s="7"/>
-      <c r="N54" s="1"/>
+      <c r="C54" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D54" s="63">
+        <v>1000</v>
+      </c>
     </row>
     <row r="55" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B55" s="15" t="s">
-        <v>90</v>
-      </c>
-      <c r="C55" s="16"/>
-      <c r="D55" s="16"/>
-      <c r="E55" s="46"/>
-      <c r="F55" s="17"/>
-      <c r="G55" s="17"/>
-      <c r="H55" s="17"/>
-      <c r="I55" s="17"/>
-      <c r="J55" s="17"/>
-      <c r="K55" s="17"/>
-      <c r="L55" s="17"/>
-      <c r="M55" s="17"/>
-      <c r="N55" s="17"/>
+      <c r="C55" s="3"/>
+      <c r="D55" s="63"/>
     </row>
     <row r="56" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B56" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C56" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="D56" s="44">
-        <v>0.13</v>
-      </c>
-      <c r="E56" s="39" t="s">
-        <v>0</v>
-      </c>
-      <c r="F56" s="57"/>
-      <c r="G56" s="57"/>
-      <c r="H56" s="57"/>
-      <c r="I56" s="57"/>
-      <c r="J56" s="57"/>
-      <c r="K56" s="57"/>
-      <c r="L56" s="57"/>
-      <c r="M56" s="57"/>
-      <c r="N56" s="1"/>
+      <c r="C56" s="3"/>
+      <c r="D56" s="63"/>
     </row>
     <row r="57" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C57" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="D57" s="55" t="s">
-        <v>105</v>
-      </c>
-      <c r="E57" s="39" t="s">
-        <v>1</v>
-      </c>
-      <c r="F57" s="57"/>
-      <c r="G57" s="57"/>
-      <c r="H57" s="57"/>
-      <c r="I57" s="57"/>
-      <c r="J57" s="57"/>
-      <c r="K57" s="57"/>
-      <c r="L57" s="57"/>
-      <c r="M57" s="57"/>
-      <c r="N57" s="1"/>
+      <c r="C57" s="3"/>
+      <c r="D57" s="63"/>
     </row>
     <row r="58" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C58" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="D58" s="49">
-        <v>0.1</v>
-      </c>
-      <c r="E58" s="39" t="s">
-        <v>2</v>
-      </c>
-      <c r="F58" s="57"/>
-      <c r="G58" s="57"/>
-      <c r="H58" s="57"/>
-      <c r="I58" s="57"/>
-      <c r="J58" s="57"/>
-      <c r="K58" s="57"/>
-      <c r="L58" s="57"/>
-      <c r="M58" s="57"/>
-      <c r="N58" s="1"/>
+      <c r="C58" s="3"/>
+      <c r="D58" s="63"/>
     </row>
     <row r="59" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C59" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D59" s="48">
-        <v>1200</v>
-      </c>
-      <c r="E59" s="35" t="s">
-        <v>3</v>
-      </c>
-      <c r="F59" s="58"/>
-      <c r="G59" s="58"/>
-      <c r="H59" s="58"/>
-      <c r="I59" s="58"/>
-      <c r="J59" s="58"/>
-      <c r="K59" s="58"/>
-      <c r="L59" s="58"/>
-      <c r="M59" s="58"/>
-      <c r="N59" s="1"/>
+      <c r="C59" s="3"/>
+      <c r="D59" s="63"/>
     </row>
     <row r="60" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C60" s="6"/>
-      <c r="N60" s="1"/>
+      <c r="C60" s="3"/>
+      <c r="D60" s="63"/>
     </row>
     <row r="61" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B61" s="15" t="s">
-        <v>112</v>
+        <v>89</v>
       </c>
       <c r="C61" s="16"/>
       <c r="D61" s="16"/>
@@ -7140,7 +7302,7 @@
         <v>66</v>
       </c>
       <c r="D63" s="55" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E63" s="39" t="s">
         <v>1</v>
@@ -7160,7 +7322,7 @@
         <v>77</v>
       </c>
       <c r="D64" s="49">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="E64" s="39" t="s">
         <v>2</v>
@@ -7175,13 +7337,11 @@
       <c r="M64" s="57"/>
       <c r="N64" s="1"/>
     </row>
-    <row r="65" spans="3:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C65" s="2" t="s">
+    <row r="65" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C65" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D65" s="48">
-        <v>1500</v>
-      </c>
+      <c r="D65" s="63"/>
       <c r="E65" s="35" t="s">
         <v>3</v>
       </c>
@@ -7195,68 +7355,232 @@
       <c r="M65" s="58"/>
       <c r="N65" s="1"/>
     </row>
-    <row r="66" spans="3:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C66" s="59" t="s">
+    <row r="66" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C66" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="D66" s="48">
-        <v>1000</v>
-      </c>
+      <c r="D66" s="63"/>
+      <c r="E66" s="35"/>
+      <c r="J66" s="7"/>
+      <c r="L66" s="7"/>
+      <c r="M66" s="7"/>
       <c r="N66" s="1"/>
     </row>
-    <row r="67" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C67" s="6"/>
-      <c r="N67" s="1"/>
-    </row>
-    <row r="68" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C68" s="6"/>
+    <row r="67" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B67" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="C67" s="16"/>
+      <c r="D67" s="16"/>
+      <c r="E67" s="46"/>
+      <c r="F67" s="17"/>
+      <c r="G67" s="17"/>
+      <c r="H67" s="17"/>
+      <c r="I67" s="17"/>
+      <c r="J67" s="17"/>
+      <c r="K67" s="17"/>
+      <c r="L67" s="17"/>
+      <c r="M67" s="17"/>
+      <c r="N67" s="17"/>
+    </row>
+    <row r="68" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B68" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C68" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D68" s="44">
+        <v>0.13</v>
+      </c>
+      <c r="E68" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="F68" s="57"/>
+      <c r="G68" s="57"/>
+      <c r="H68" s="57"/>
+      <c r="I68" s="57"/>
+      <c r="J68" s="57"/>
+      <c r="K68" s="57"/>
+      <c r="L68" s="57"/>
+      <c r="M68" s="57"/>
       <c r="N68" s="1"/>
     </row>
-    <row r="69" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C69" s="6"/>
+    <row r="69" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C69" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D69" s="55" t="s">
+        <v>105</v>
+      </c>
+      <c r="E69" s="39" t="s">
+        <v>1</v>
+      </c>
+      <c r="F69" s="57"/>
+      <c r="G69" s="57"/>
+      <c r="H69" s="57"/>
+      <c r="I69" s="57"/>
+      <c r="J69" s="57"/>
+      <c r="K69" s="57"/>
+      <c r="L69" s="57"/>
+      <c r="M69" s="57"/>
       <c r="N69" s="1"/>
     </row>
-    <row r="70" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C70" s="6"/>
+    <row r="70" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C70" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D70" s="49">
+        <v>0.1</v>
+      </c>
+      <c r="E70" s="39" t="s">
+        <v>2</v>
+      </c>
+      <c r="F70" s="57"/>
+      <c r="G70" s="57"/>
+      <c r="H70" s="57"/>
+      <c r="I70" s="57"/>
+      <c r="J70" s="57"/>
+      <c r="K70" s="57"/>
+      <c r="L70" s="57"/>
+      <c r="M70" s="57"/>
       <c r="N70" s="1"/>
     </row>
-    <row r="71" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C71" s="6"/>
+    <row r="71" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C71" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D71" s="63"/>
+      <c r="E71" s="35" t="s">
+        <v>3</v>
+      </c>
+      <c r="F71" s="58"/>
+      <c r="G71" s="58"/>
+      <c r="H71" s="58"/>
+      <c r="I71" s="58"/>
+      <c r="J71" s="58"/>
+      <c r="K71" s="58"/>
+      <c r="L71" s="58"/>
+      <c r="M71" s="58"/>
       <c r="N71" s="1"/>
     </row>
-    <row r="72" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C72" s="6"/>
+    <row r="72" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C72" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="D72" s="63"/>
       <c r="N72" s="1"/>
     </row>
-    <row r="73" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C73" s="6"/>
-      <c r="N73" s="1"/>
-    </row>
-    <row r="74" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C74" s="6"/>
+    <row r="73" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B73" s="15" t="s">
+        <v>112</v>
+      </c>
+      <c r="C73" s="16"/>
+      <c r="D73" s="16"/>
+      <c r="E73" s="46"/>
+      <c r="F73" s="17"/>
+      <c r="G73" s="17"/>
+      <c r="H73" s="17"/>
+      <c r="I73" s="17"/>
+      <c r="J73" s="17"/>
+      <c r="K73" s="17"/>
+      <c r="L73" s="17"/>
+      <c r="M73" s="17"/>
+      <c r="N73" s="17"/>
+    </row>
+    <row r="74" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B74" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D74" s="44">
+        <v>0.13</v>
+      </c>
+      <c r="E74" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="F74" s="57"/>
+      <c r="G74" s="57"/>
+      <c r="H74" s="57"/>
+      <c r="I74" s="57"/>
+      <c r="J74" s="57"/>
+      <c r="K74" s="57"/>
+      <c r="L74" s="57"/>
+      <c r="M74" s="57"/>
       <c r="N74" s="1"/>
     </row>
-    <row r="75" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C75" s="6"/>
+    <row r="75" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C75" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D75" s="55" t="s">
+        <v>105</v>
+      </c>
+      <c r="E75" s="39" t="s">
+        <v>1</v>
+      </c>
+      <c r="F75" s="57"/>
+      <c r="G75" s="57"/>
+      <c r="H75" s="57"/>
+      <c r="I75" s="57"/>
+      <c r="J75" s="57"/>
+      <c r="K75" s="57"/>
+      <c r="L75" s="57"/>
+      <c r="M75" s="57"/>
       <c r="N75" s="1"/>
     </row>
-    <row r="76" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C76" s="6"/>
+    <row r="76" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C76" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D76" s="49">
+        <v>0.1</v>
+      </c>
+      <c r="E76" s="39" t="s">
+        <v>2</v>
+      </c>
+      <c r="F76" s="57"/>
+      <c r="G76" s="57"/>
+      <c r="H76" s="57"/>
+      <c r="I76" s="57"/>
+      <c r="J76" s="57"/>
+      <c r="K76" s="57"/>
+      <c r="L76" s="57"/>
+      <c r="M76" s="57"/>
       <c r="N76" s="1"/>
     </row>
-    <row r="77" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C77" s="6"/>
+    <row r="77" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C77" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D77" s="63"/>
+      <c r="E77" s="35" t="s">
+        <v>3</v>
+      </c>
+      <c r="F77" s="58"/>
+      <c r="G77" s="58"/>
+      <c r="H77" s="58"/>
+      <c r="I77" s="58"/>
+      <c r="J77" s="58"/>
+      <c r="K77" s="58"/>
+      <c r="L77" s="58"/>
+      <c r="M77" s="58"/>
       <c r="N77" s="1"/>
     </row>
-    <row r="78" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C78" s="6"/>
+    <row r="78" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C78" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="D78" s="63"/>
       <c r="N78" s="1"/>
     </row>
-    <row r="79" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C79" s="6"/>
       <c r="N79" s="1"/>
     </row>
-    <row r="80" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C80" s="6"/>
       <c r="N80" s="1"/>
     </row>
@@ -7324,90 +7648,137 @@
       <c r="C96" s="6"/>
       <c r="N96" s="1"/>
     </row>
-    <row r="97" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="97" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C97" s="6"/>
       <c r="N97" s="1"/>
     </row>
-    <row r="98" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="98" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C98" s="6"/>
       <c r="N98" s="1"/>
     </row>
-    <row r="99" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="99" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C99" s="6"/>
       <c r="N99" s="1"/>
     </row>
-    <row r="100" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="100" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C100" s="6"/>
       <c r="N100" s="1"/>
     </row>
-    <row r="101" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="101" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C101" s="6"/>
       <c r="N101" s="1"/>
     </row>
-    <row r="102" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="102" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C102" s="6"/>
       <c r="N102" s="1"/>
     </row>
-    <row r="103" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="103" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C103" s="6"/>
       <c r="N103" s="1"/>
     </row>
-    <row r="104" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="104" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C104" s="6"/>
       <c r="N104" s="1"/>
     </row>
-    <row r="105" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="105" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C105" s="6"/>
       <c r="N105" s="1"/>
     </row>
-    <row r="106" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="E106" s="35"/>
+    <row r="106" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C106" s="6"/>
       <c r="N106" s="1"/>
     </row>
-    <row r="107" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="107" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C107" s="6"/>
       <c r="N107" s="1"/>
     </row>
-    <row r="108" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B108" s="22" t="s">
+    <row r="108" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C108" s="6"/>
+      <c r="N108" s="1"/>
+    </row>
+    <row r="109" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C109" s="6"/>
+      <c r="N109" s="1"/>
+    </row>
+    <row r="110" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C110" s="6"/>
+      <c r="N110" s="1"/>
+    </row>
+    <row r="111" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C111" s="6"/>
+      <c r="N111" s="1"/>
+    </row>
+    <row r="112" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C112" s="6"/>
+      <c r="N112" s="1"/>
+    </row>
+    <row r="113" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="C113" s="6"/>
+      <c r="N113" s="1"/>
+    </row>
+    <row r="114" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="C114" s="6"/>
+      <c r="N114" s="1"/>
+    </row>
+    <row r="115" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="C115" s="6"/>
+      <c r="N115" s="1"/>
+    </row>
+    <row r="116" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="N116" s="1"/>
+    </row>
+    <row r="117" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="N117" s="1"/>
+    </row>
+    <row r="118" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="E118" s="35"/>
+      <c r="N118" s="1"/>
+    </row>
+    <row r="119" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="N119" s="1"/>
+    </row>
+    <row r="120" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B120" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="C108" s="23"/>
-      <c r="D108" s="23"/>
-      <c r="E108" s="47"/>
-      <c r="F108" s="24"/>
-      <c r="G108" s="24"/>
-      <c r="H108" s="24"/>
-      <c r="I108" s="24"/>
-      <c r="J108" s="24"/>
-      <c r="K108" s="24"/>
-      <c r="L108" s="25"/>
-      <c r="M108" s="43"/>
-    </row>
-    <row r="109" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B109"/>
-      <c r="C109"/>
-      <c r="D109"/>
-      <c r="E109" s="3"/>
-      <c r="F109"/>
-      <c r="G109"/>
-      <c r="H109"/>
-      <c r="I109"/>
-      <c r="J109"/>
-      <c r="K109"/>
-      <c r="L109"/>
-      <c r="M109"/>
-    </row>
-    <row r="124" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P124" s="3"/>
-      <c r="Q124"/>
-      <c r="R124"/>
-    </row>
-    <row r="125" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="Q125"/>
-      <c r="R125"/>
+      <c r="C120" s="23"/>
+      <c r="D120" s="23"/>
+      <c r="E120" s="47"/>
+      <c r="F120" s="24"/>
+      <c r="G120" s="24"/>
+      <c r="H120" s="24"/>
+      <c r="I120" s="24"/>
+      <c r="J120" s="24"/>
+      <c r="K120" s="24"/>
+      <c r="L120" s="25"/>
+      <c r="M120" s="43"/>
+    </row>
+    <row r="121" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B121"/>
+      <c r="C121"/>
+      <c r="D121"/>
+      <c r="E121" s="3"/>
+      <c r="F121"/>
+      <c r="G121"/>
+      <c r="H121"/>
+      <c r="I121"/>
+      <c r="J121"/>
+      <c r="K121"/>
+      <c r="L121"/>
+      <c r="M121"/>
+    </row>
+    <row r="136" spans="16:18" x14ac:dyDescent="0.25">
+      <c r="P136" s="3"/>
+      <c r="Q136"/>
+      <c r="R136"/>
+    </row>
+    <row r="137" spans="16:18" x14ac:dyDescent="0.25">
+      <c r="Q137"/>
+      <c r="R137"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -7417,7 +7788,7 @@
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J2" sqref="J2"/>
+      <selection pane="bottomLeft" activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7670,11 +8041,17 @@
       <c r="M20"/>
     </row>
     <row r="21" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C21" s="59" t="s">
+        <v>113</v>
+      </c>
       <c r="J21" s="3"/>
       <c r="L21" s="3"/>
       <c r="M21"/>
     </row>
     <row r="22" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="C22" s="59" t="s">
+        <v>114</v>
+      </c>
       <c r="J22" s="3"/>
       <c r="L22" s="3"/>
       <c r="M22"/>
@@ -7791,4 +8168,95 @@
   <pageSetup orientation="portrait" r:id="rId2"/>
   <drawing r:id="rId3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FF9F3D8-EE75-4BA9-AEF3-53D4AB9C675D}">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="45.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="52.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="68.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="60"/>
+      <c r="B2" s="60" t="s">
+        <v>123</v>
+      </c>
+      <c r="C2" s="64" t="s">
+        <v>122</v>
+      </c>
+      <c r="D2" s="60">
+        <v>2022</v>
+      </c>
+      <c r="E2" s="60"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="60"/>
+      <c r="B3" s="60" t="s">
+        <v>124</v>
+      </c>
+      <c r="C3" s="64" t="s">
+        <v>125</v>
+      </c>
+      <c r="D3" s="60">
+        <v>2007</v>
+      </c>
+      <c r="E3" s="60"/>
+    </row>
+    <row r="4" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A4" s="60"/>
+      <c r="B4" s="60" t="s">
+        <v>129</v>
+      </c>
+      <c r="C4" s="64" t="s">
+        <v>130</v>
+      </c>
+      <c r="D4" s="60">
+        <v>2011</v>
+      </c>
+      <c r="E4" s="65" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" s="60" customFormat="1" ht="165" x14ac:dyDescent="0.25">
+      <c r="A5" s="60" t="s">
+        <v>131</v>
+      </c>
+      <c r="B5" s="60" t="s">
+        <v>127</v>
+      </c>
+      <c r="C5" s="64" t="s">
+        <v>126</v>
+      </c>
+      <c r="D5" s="60">
+        <v>2020</v>
+      </c>
+      <c r="E5" s="65" t="s">
+        <v>128</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{5450ADFF-AC80-4464-AED6-6C64D2F3195C}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{4A9B6726-94CC-4E39-9CB3-411D784423FB}"/>
+    <hyperlink ref="C5" r:id="rId3" xr:uid="{A4F1E726-24DD-4B36-A6D9-46BBCCC6C578}"/>
+    <hyperlink ref="C4" r:id="rId4" xr:uid="{4D7706F1-DA38-4791-A40E-6329AC8CA156}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
High noise experiments conducted for PHM C01 data set
</commit_message>
<xml_diff>
--- a/analysis/Analysis_Experiments_V5_13-May-2023.xlsx
+++ b/analysis/Analysis_Experiments_V5_13-May-2023.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Rajesh\ResearchLab\RL_for_PdM\REINFORCE_Tool_Replace_Policy\analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{042ABF74-40FC-4957-A517-88B69CDC25E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4248E27B-2409-46E8-AE46-71CAACF456AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="506" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Simulated Env. Expts." sheetId="9" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="538" uniqueCount="142">
   <si>
     <t>A2C</t>
   </si>
@@ -607,9 +607,6 @@
   </si>
   <si>
     <t>Weigthed. Precision oriented F-Beta scores</t>
-  </si>
-  <si>
-    <t>C-06. High noise and break-down. 1.5k episodes. 1k termination</t>
   </si>
   <si>
     <t>RECALL error was 1.0</t>
@@ -760,6 +757,75 @@
   <si>
     <t>C-06. No noise or break-down. Increase Episodes and Termination parmeters</t>
   </si>
+  <si>
+    <t>High precision. But low F-scores</t>
+  </si>
+  <si>
+    <t>C-06. Low noise and break-down - Expt.2 - 2k/1k</t>
+  </si>
+  <si>
+    <t>*** All parameters improved.</t>
+  </si>
+  <si>
+    <t>GOLD</t>
+  </si>
+  <si>
+    <t>Good example</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">C-06. High noise and break-down. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>LOWER DOWN</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 1k episodes and </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>same</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 1k termination</t>
+    </r>
+  </si>
+  <si>
+    <t>Lower ep./term</t>
+  </si>
 </sst>
 </file>
 
@@ -769,7 +835,7 @@
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.00000"/>
   </numFmts>
-  <fonts count="38" x14ac:knownFonts="1">
+  <fonts count="39" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1061,8 +1127,17 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FFC00000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="39">
+  <fills count="40">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1278,8 +1353,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF8F280"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="14">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -1438,6 +1519,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1485,7 +1581,7 @@
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1639,6 +1735,13 @@
     <xf numFmtId="1" fontId="35" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="36" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="37" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="39" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="37" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="44">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1690,6 +1793,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFF8F280"/>
       <color rgb="FF0000FF"/>
       <color rgb="FF3333FF"/>
     </mruColors>
@@ -2066,6 +2170,161 @@
 </file>
 
 <file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>95249</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>238125</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>200025</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{795A5FC3-5F3B-BBCD-8ED6-745C0B7592B3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10048874" y="17449800"/>
+          <a:ext cx="3619501" cy="1447800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>228599</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>41910</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>352423</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>60960</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CC149416-FB0C-1903-B17B-862C8DA6B325}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13782674" y="17501235"/>
+          <a:ext cx="1904999" cy="762000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>219076</xdr:colOff>
+      <xdr:row>71</xdr:row>
+      <xdr:rowOff>219075</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>366713</xdr:colOff>
+      <xdr:row>75</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CC96FF48-8565-08C8-03E3-697406C515F7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13773151" y="18173700"/>
+          <a:ext cx="1928812" cy="771525"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
@@ -3789,8 +4048,8 @@
   <dimension ref="A2:W87"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F53" sqref="F53:M53"/>
+      <pane ySplit="4" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="S12" sqref="S12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4042,7 +4301,7 @@
         <v>0.53500000000000003</v>
       </c>
     </row>
-    <row r="9" spans="1:20" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C9" s="2" t="s">
         <v>51</v>
       </c>
@@ -4084,9 +4343,9 @@
       <c r="S9" s="53"/>
       <c r="T9" s="53"/>
     </row>
-    <row r="10" spans="1:20" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C10" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D10" s="48">
         <v>800</v>
@@ -4096,6 +4355,12 @@
       </c>
       <c r="Q10" s="14">
         <v>1.234</v>
+      </c>
+      <c r="S10" s="70" t="s">
+        <v>138</v>
+      </c>
+      <c r="T10" s="3" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="11" spans="1:20" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -4289,7 +4554,7 @@
     </row>
     <row r="16" spans="1:20" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C16" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D16" s="48">
         <v>800</v>
@@ -4504,7 +4769,7 @@
     </row>
     <row r="22" spans="1:23" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C22" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D22" s="48">
         <v>800</v>
@@ -4734,7 +4999,7 @@
     </row>
     <row r="29" spans="1:23" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C29" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D29" s="48">
         <v>800</v>
@@ -4932,7 +5197,7 @@
     </row>
     <row r="35" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C35" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D35" s="48">
         <v>800</v>
@@ -5109,7 +5374,7 @@
     </row>
     <row r="41" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C41" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D41" s="48">
         <v>800</v>
@@ -5327,13 +5592,13 @@
     </row>
     <row r="48" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C48" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D48" s="48">
         <v>800</v>
       </c>
     </row>
-    <row r="49" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B49" s="15" t="s">
         <v>89</v>
       </c>
@@ -5350,7 +5615,7 @@
       <c r="M49" s="17"/>
       <c r="N49" s="17"/>
     </row>
-    <row r="50" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B50" s="3" t="s">
         <v>10</v>
       </c>
@@ -5389,7 +5654,7 @@
       </c>
       <c r="N50" s="1"/>
     </row>
-    <row r="51" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C51" s="2" t="s">
         <v>66</v>
       </c>
@@ -5425,7 +5690,7 @@
       </c>
       <c r="N51" s="1"/>
     </row>
-    <row r="52" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C52" s="2" t="s">
         <v>77</v>
       </c>
@@ -5461,7 +5726,7 @@
       </c>
       <c r="N52" s="1"/>
     </row>
-    <row r="53" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C53" s="2" t="s">
         <v>51</v>
       </c>
@@ -5497,9 +5762,9 @@
       </c>
       <c r="N53" s="1"/>
     </row>
-    <row r="54" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C54" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D54" s="48">
         <v>800</v>
@@ -5510,7 +5775,7 @@
       <c r="M54" s="7"/>
       <c r="N54" s="1"/>
     </row>
-    <row r="55" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B55" s="15" t="s">
         <v>90</v>
       </c>
@@ -5527,7 +5792,7 @@
       <c r="M55" s="17"/>
       <c r="N55" s="17"/>
     </row>
-    <row r="56" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B56" s="3" t="s">
         <v>10</v>
       </c>
@@ -5566,7 +5831,7 @@
       </c>
       <c r="N56" s="1"/>
     </row>
-    <row r="57" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C57" s="2" t="s">
         <v>66</v>
       </c>
@@ -5602,7 +5867,7 @@
       </c>
       <c r="N57" s="1"/>
     </row>
-    <row r="58" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C58" s="2" t="s">
         <v>77</v>
       </c>
@@ -5638,7 +5903,7 @@
       </c>
       <c r="N58" s="1"/>
     </row>
-    <row r="59" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C59" s="2" t="s">
         <v>51</v>
       </c>
@@ -5673,10 +5938,10 @@
         <v>0.34</v>
       </c>
       <c r="N59" s="42" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="60" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="60" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C60" s="2" t="s">
         <v>97</v>
       </c>
@@ -5684,23 +5949,26 @@
         <v>800</v>
       </c>
       <c r="E60" s="35"/>
-      <c r="F60" s="9"/>
-      <c r="G60" s="9"/>
-      <c r="H60" s="9"/>
-      <c r="I60" s="9"/>
-      <c r="J60" s="9"/>
-      <c r="K60" s="9"/>
-      <c r="L60" s="56"/>
-      <c r="M60" s="9"/>
-      <c r="N60" s="42"/>
-    </row>
-    <row r="61" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F60" s="35"/>
+      <c r="G60" s="35"/>
+      <c r="H60" s="35"/>
+      <c r="I60" s="35"/>
+      <c r="J60" s="35"/>
+      <c r="K60" s="35"/>
+      <c r="L60" s="35"/>
+      <c r="M60" s="35"/>
+      <c r="N60" s="35"/>
+    </row>
+    <row r="61" spans="1:14" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C61" s="6"/>
       <c r="N61" s="1"/>
     </row>
-    <row r="62" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:14" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="70" t="s">
+        <v>138</v>
+      </c>
       <c r="B62" s="15" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C62" s="16"/>
       <c r="D62" s="16"/>
@@ -5715,7 +5983,7 @@
       <c r="M62" s="17"/>
       <c r="N62" s="17"/>
     </row>
-    <row r="63" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B63" s="3" t="s">
         <v>10</v>
       </c>
@@ -5753,7 +6021,7 @@
         <v>0.375</v>
       </c>
     </row>
-    <row r="64" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C64" s="2" t="s">
         <v>66</v>
       </c>
@@ -5858,7 +6126,7 @@
         <v>0.20499999999999999</v>
       </c>
       <c r="N66" s="42" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="67" spans="2:22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -5879,7 +6147,7 @@
     </row>
     <row r="70" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B70" s="22" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C70" s="23"/>
       <c r="D70" s="23"/>
@@ -5932,11 +6200,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE699FEF-4516-4E3F-8EE7-4192FF715912}">
-  <dimension ref="A2:W137"/>
+  <dimension ref="A2:W140"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F54" sqref="F54"/>
+      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M21" sqref="M21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5944,7 +6212,7 @@
     <col min="2" max="2" width="7.7109375" style="3" customWidth="1"/>
     <col min="3" max="3" width="14.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.140625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="15.28515625" style="39" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" style="39" bestFit="1" customWidth="1"/>
     <col min="6" max="13" width="9.42578125" style="1" customWidth="1"/>
     <col min="14" max="14" width="17.28515625" customWidth="1"/>
     <col min="15" max="15" width="8.140625" customWidth="1"/>
@@ -6062,14 +6330,30 @@
       <c r="E6" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="F6" s="57"/>
-      <c r="G6" s="57"/>
-      <c r="H6" s="57"/>
-      <c r="I6" s="57"/>
-      <c r="J6" s="57"/>
-      <c r="K6" s="57"/>
-      <c r="L6" s="57"/>
-      <c r="M6" s="57"/>
+      <c r="F6" s="57">
+        <v>0.51241999999999999</v>
+      </c>
+      <c r="G6" s="57">
+        <v>0.46500000000000002</v>
+      </c>
+      <c r="H6" s="57">
+        <v>0.49359999999999998</v>
+      </c>
+      <c r="I6" s="57">
+        <v>0.48218699999999998</v>
+      </c>
+      <c r="J6" s="57">
+        <v>0.474574</v>
+      </c>
+      <c r="K6" s="57">
+        <v>0.56523800000000002</v>
+      </c>
+      <c r="L6" s="57">
+        <v>0.49329000000000001</v>
+      </c>
+      <c r="M6" s="57">
+        <v>0.53500000000000003</v>
+      </c>
       <c r="P6" s="3" t="s">
         <v>92</v>
       </c>
@@ -6097,14 +6381,30 @@
       <c r="E7" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="F7" s="57"/>
-      <c r="G7" s="57"/>
-      <c r="H7" s="57"/>
-      <c r="I7" s="57"/>
-      <c r="J7" s="57"/>
-      <c r="K7" s="57"/>
-      <c r="L7" s="57"/>
-      <c r="M7" s="57"/>
+      <c r="F7" s="57">
+        <v>0.53688100000000005</v>
+      </c>
+      <c r="G7" s="57">
+        <v>0.43</v>
+      </c>
+      <c r="H7" s="57">
+        <v>0.26383299999999998</v>
+      </c>
+      <c r="I7" s="57">
+        <v>0.26130799999999998</v>
+      </c>
+      <c r="J7" s="57">
+        <v>0.27624300000000002</v>
+      </c>
+      <c r="K7" s="57">
+        <v>0.97478399999999998</v>
+      </c>
+      <c r="L7" s="57">
+        <v>0</v>
+      </c>
+      <c r="M7" s="57">
+        <v>0.56999999999999995</v>
+      </c>
       <c r="P7" s="8" t="s">
         <v>93</v>
       </c>
@@ -6131,31 +6431,65 @@
       <c r="E8" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="F8" s="57"/>
-      <c r="G8" s="57"/>
-      <c r="H8" s="57"/>
-      <c r="I8" s="57"/>
-      <c r="J8" s="57"/>
-      <c r="K8" s="57"/>
-      <c r="L8" s="57"/>
-      <c r="M8" s="57"/>
-    </row>
-    <row r="9" spans="1:20" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C9" s="3" t="s">
+      <c r="F8" s="57">
+        <v>0.52627199999999996</v>
+      </c>
+      <c r="G8" s="57">
+        <v>0.46</v>
+      </c>
+      <c r="H8" s="57">
+        <v>0.49975999999999998</v>
+      </c>
+      <c r="I8" s="57">
+        <v>0.483844</v>
+      </c>
+      <c r="J8" s="57">
+        <v>0.47327900000000001</v>
+      </c>
+      <c r="K8" s="57">
+        <v>0.56609900000000002</v>
+      </c>
+      <c r="L8" s="57">
+        <v>0.49157000000000001</v>
+      </c>
+      <c r="M8" s="57">
+        <v>0.54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C9" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="D9" s="63"/>
+      <c r="D9" s="63">
+        <v>1200</v>
+      </c>
       <c r="E9" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="F9" s="58"/>
-      <c r="G9" s="58"/>
-      <c r="H9" s="58"/>
-      <c r="I9" s="58"/>
-      <c r="J9" s="58"/>
-      <c r="K9" s="58"/>
-      <c r="L9" s="58"/>
-      <c r="M9" s="58"/>
+      <c r="F9" s="9">
+        <v>0.83469800000000005</v>
+      </c>
+      <c r="G9" s="9">
+        <v>0.755</v>
+      </c>
+      <c r="H9" s="9">
+        <v>0.78266500000000006</v>
+      </c>
+      <c r="I9" s="9">
+        <v>0.75824999999999998</v>
+      </c>
+      <c r="J9" s="9">
+        <v>0.74578999999999995</v>
+      </c>
+      <c r="K9" s="9">
+        <v>0.42594700000000002</v>
+      </c>
+      <c r="L9" s="9">
+        <v>2.2856999999999999E-2</v>
+      </c>
+      <c r="M9" s="9">
+        <v>0.245</v>
+      </c>
       <c r="P9" s="51" t="s">
         <v>21</v>
       </c>
@@ -6164,16 +6498,24 @@
       <c r="S9" s="53"/>
       <c r="T9" s="53"/>
     </row>
-    <row r="10" spans="1:20" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C10" s="3" t="s">
+    <row r="10" spans="1:20" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C10" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="D10" s="63"/>
+      <c r="D10" s="63">
+        <v>1000</v>
+      </c>
       <c r="P10" s="3" t="s">
         <v>19</v>
       </c>
       <c r="Q10" s="14">
         <v>1.234</v>
+      </c>
+      <c r="S10" s="70" t="s">
+        <v>138</v>
+      </c>
+      <c r="T10" s="3" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="11" spans="1:20" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -6212,14 +6554,30 @@
       <c r="E12" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="F12" s="57"/>
-      <c r="G12" s="57"/>
-      <c r="H12" s="57"/>
-      <c r="I12" s="57"/>
-      <c r="J12" s="57"/>
-      <c r="K12" s="57"/>
-      <c r="L12" s="57"/>
-      <c r="M12" s="57"/>
+      <c r="F12" s="57">
+        <v>0.52624700000000002</v>
+      </c>
+      <c r="G12" s="57">
+        <v>0.44</v>
+      </c>
+      <c r="H12" s="57">
+        <v>0.47889999999999999</v>
+      </c>
+      <c r="I12" s="57">
+        <v>0.454233</v>
+      </c>
+      <c r="J12" s="57">
+        <v>0.44014199999999998</v>
+      </c>
+      <c r="K12" s="57">
+        <v>0.66026200000000002</v>
+      </c>
+      <c r="L12" s="57">
+        <v>0.37605300000000003</v>
+      </c>
+      <c r="M12" s="57">
+        <v>0.56000000000000005</v>
+      </c>
       <c r="N12" s="1"/>
       <c r="P12" s="3" t="s">
         <v>108</v>
@@ -6238,14 +6596,30 @@
       <c r="E13" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="F13" s="57"/>
-      <c r="G13" s="57"/>
-      <c r="H13" s="57"/>
-      <c r="I13" s="57"/>
-      <c r="J13" s="57"/>
-      <c r="K13" s="57"/>
-      <c r="L13" s="57"/>
-      <c r="M13" s="57"/>
+      <c r="F13" s="57">
+        <v>0.26966699999999999</v>
+      </c>
+      <c r="G13" s="57">
+        <v>0.36</v>
+      </c>
+      <c r="H13" s="57">
+        <v>0.21025199999999999</v>
+      </c>
+      <c r="I13" s="57">
+        <v>0.21374099999999999</v>
+      </c>
+      <c r="J13" s="57">
+        <v>0.22736100000000001</v>
+      </c>
+      <c r="K13" s="57">
+        <v>0.97592599999999996</v>
+      </c>
+      <c r="L13" s="67">
+        <v>0.10425</v>
+      </c>
+      <c r="M13" s="57">
+        <v>0.64</v>
+      </c>
       <c r="N13" s="1"/>
     </row>
     <row r="14" spans="1:20" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -6258,14 +6632,30 @@
       <c r="E14" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="F14" s="57"/>
-      <c r="G14" s="57"/>
-      <c r="H14" s="57"/>
-      <c r="I14" s="57"/>
-      <c r="J14" s="57"/>
-      <c r="K14" s="57"/>
-      <c r="L14" s="57"/>
-      <c r="M14" s="57"/>
+      <c r="F14" s="57">
+        <v>0.54367100000000002</v>
+      </c>
+      <c r="G14" s="57">
+        <v>0.52</v>
+      </c>
+      <c r="H14" s="57">
+        <v>0.53242699999999998</v>
+      </c>
+      <c r="I14" s="57">
+        <v>0.52595499999999995</v>
+      </c>
+      <c r="J14" s="57">
+        <v>0.52196200000000004</v>
+      </c>
+      <c r="K14" s="57">
+        <v>0.51052900000000001</v>
+      </c>
+      <c r="L14" s="57">
+        <v>0.44590800000000003</v>
+      </c>
+      <c r="M14" s="57">
+        <v>0.48</v>
+      </c>
       <c r="N14" s="1"/>
       <c r="P14" s="51" t="s">
         <v>94</v>
@@ -6276,34 +6666,54 @@
       <c r="T14" s="53"/>
     </row>
     <row r="15" spans="1:20" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="D15" s="63"/>
+      <c r="D15" s="63">
+        <v>1800</v>
+      </c>
       <c r="E15" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="F15" s="58"/>
-      <c r="G15" s="58"/>
-      <c r="H15" s="58"/>
-      <c r="I15" s="58"/>
-      <c r="J15" s="58"/>
-      <c r="K15" s="58"/>
-      <c r="L15" s="58"/>
-      <c r="M15" s="58"/>
+      <c r="F15" s="9">
+        <v>0.73341800000000001</v>
+      </c>
+      <c r="G15" s="9">
+        <v>0.73</v>
+      </c>
+      <c r="H15" s="9">
+        <v>0.71030499999999996</v>
+      </c>
+      <c r="I15" s="9">
+        <v>0.70309500000000003</v>
+      </c>
+      <c r="J15" s="9">
+        <v>0.70234399999999997</v>
+      </c>
+      <c r="K15" s="9">
+        <v>8.1398999999999999E-2</v>
+      </c>
+      <c r="L15" s="57">
+        <v>0.64204399999999995</v>
+      </c>
+      <c r="M15" s="9">
+        <v>0.27</v>
+      </c>
       <c r="N15" s="1"/>
       <c r="P15" s="3" t="s">
         <v>95</v>
       </c>
       <c r="Q15" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="16" spans="1:20" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="D16" s="63"/>
+      <c r="D16" s="63">
+        <v>1500</v>
+      </c>
       <c r="E16" s="35"/>
       <c r="J16" s="7"/>
       <c r="L16" s="7"/>
@@ -6313,7 +6723,7 @@
         <v>100</v>
       </c>
       <c r="Q16" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="17" spans="1:23" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -6333,7 +6743,7 @@
       <c r="M17" s="17"/>
       <c r="N17" s="17"/>
       <c r="Q17" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="18" spans="1:23" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -6349,14 +6759,30 @@
       <c r="E18" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="F18" s="57"/>
-      <c r="G18" s="57"/>
-      <c r="H18" s="57"/>
-      <c r="I18" s="57"/>
-      <c r="J18" s="57"/>
-      <c r="K18" s="57"/>
-      <c r="L18" s="57"/>
-      <c r="M18" s="57"/>
+      <c r="F18" s="57">
+        <v>0.51565399999999995</v>
+      </c>
+      <c r="G18" s="57">
+        <v>0.48499999999999999</v>
+      </c>
+      <c r="H18" s="57">
+        <v>0.50102400000000002</v>
+      </c>
+      <c r="I18" s="57">
+        <v>0.49265100000000001</v>
+      </c>
+      <c r="J18" s="57">
+        <v>0.48751</v>
+      </c>
+      <c r="K18" s="57">
+        <v>0.56136699999999995</v>
+      </c>
+      <c r="L18" s="57">
+        <v>0.45231700000000002</v>
+      </c>
+      <c r="M18" s="57">
+        <v>0.51500000000000001</v>
+      </c>
       <c r="N18" s="1"/>
       <c r="P18" s="3" t="s">
         <v>51</v>
@@ -6375,14 +6801,30 @@
       <c r="E19" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="F19" s="57"/>
-      <c r="G19" s="57"/>
-      <c r="H19" s="57"/>
-      <c r="I19" s="57"/>
-      <c r="J19" s="57"/>
-      <c r="K19" s="57"/>
-      <c r="L19" s="57"/>
-      <c r="M19" s="57"/>
+      <c r="F19" s="57">
+        <v>0.37508599999999997</v>
+      </c>
+      <c r="G19" s="57">
+        <v>0.35499999999999998</v>
+      </c>
+      <c r="H19" s="57">
+        <v>0.24263899999999999</v>
+      </c>
+      <c r="I19" s="57">
+        <v>0.23191999999999999</v>
+      </c>
+      <c r="J19" s="57">
+        <v>0.23852999999999999</v>
+      </c>
+      <c r="K19" s="57">
+        <v>0.95913899999999996</v>
+      </c>
+      <c r="L19" s="67">
+        <v>0.12460599999999999</v>
+      </c>
+      <c r="M19" s="57">
+        <v>0.64500000000000002</v>
+      </c>
       <c r="N19" s="1"/>
       <c r="P19" s="3" t="s">
         <v>97</v>
@@ -6396,19 +6838,35 @@
         <v>77</v>
       </c>
       <c r="D20" s="49">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="E20" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="F20" s="57"/>
-      <c r="G20" s="57"/>
-      <c r="H20" s="57"/>
-      <c r="I20" s="57"/>
-      <c r="J20" s="57"/>
-      <c r="K20" s="57"/>
-      <c r="L20" s="57"/>
-      <c r="M20" s="57"/>
+      <c r="F20" s="57">
+        <v>0.55005199999999999</v>
+      </c>
+      <c r="G20" s="57">
+        <v>0.505</v>
+      </c>
+      <c r="H20" s="57">
+        <v>0.53109399999999996</v>
+      </c>
+      <c r="I20" s="57">
+        <v>0.51975000000000005</v>
+      </c>
+      <c r="J20" s="57">
+        <v>0.512378</v>
+      </c>
+      <c r="K20" s="57">
+        <v>0.53175300000000003</v>
+      </c>
+      <c r="L20" s="57">
+        <v>0.44875900000000002</v>
+      </c>
+      <c r="M20" s="57">
+        <v>0.495</v>
+      </c>
       <c r="N20" s="1"/>
       <c r="P20" s="3" t="s">
         <v>56</v>
@@ -6418,21 +6876,39 @@
       </c>
     </row>
     <row r="21" spans="1:23" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C21" s="3" t="s">
+      <c r="C21" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="D21" s="63"/>
+      <c r="D21" s="63">
+        <v>1000</v>
+      </c>
       <c r="E21" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="F21" s="58"/>
-      <c r="G21" s="58"/>
-      <c r="H21" s="58"/>
-      <c r="I21" s="58"/>
-      <c r="J21" s="58"/>
-      <c r="K21" s="58"/>
-      <c r="L21" s="58"/>
-      <c r="M21" s="58"/>
+      <c r="F21" s="9">
+        <v>0.73857799999999996</v>
+      </c>
+      <c r="G21" s="9">
+        <v>0.73</v>
+      </c>
+      <c r="H21" s="9">
+        <v>0.676925</v>
+      </c>
+      <c r="I21" s="9">
+        <v>0.66550200000000004</v>
+      </c>
+      <c r="J21" s="9">
+        <v>0.66783700000000001</v>
+      </c>
+      <c r="K21" s="9">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="L21" s="57">
+        <v>0.80558799999999997</v>
+      </c>
+      <c r="M21" s="9">
+        <v>0.27</v>
+      </c>
       <c r="N21" s="1"/>
       <c r="P21" s="3" t="s">
         <v>58</v>
@@ -6443,10 +6919,12 @@
       <c r="R21"/>
     </row>
     <row r="22" spans="1:23" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C22" s="3" t="s">
+      <c r="C22" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="D22" s="63"/>
+      <c r="D22" s="63">
+        <v>800</v>
+      </c>
       <c r="J22" s="7"/>
       <c r="L22" s="7"/>
       <c r="M22" s="7"/>
@@ -6594,7 +7072,7 @@
       <c r="C28" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="D28" s="48"/>
+      <c r="D28" s="63"/>
       <c r="E28" s="35" t="s">
         <v>3</v>
       </c>
@@ -6610,6 +7088,10 @@
       <c r="R28"/>
     </row>
     <row r="29" spans="1:23" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C29" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D29" s="63"/>
       <c r="Q29"/>
       <c r="R29"/>
     </row>
@@ -7060,9 +7542,9 @@
         <v>800</v>
       </c>
     </row>
-    <row r="49" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B49" s="15" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C49" s="16"/>
       <c r="D49" s="16"/>
@@ -7077,7 +7559,7 @@
       <c r="M49" s="17"/>
       <c r="N49" s="17"/>
     </row>
-    <row r="50" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B50" s="3" t="s">
         <v>10</v>
       </c>
@@ -7116,7 +7598,7 @@
       </c>
       <c r="N50" s="1"/>
     </row>
-    <row r="51" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B51" s="2"/>
       <c r="C51" s="2" t="s">
         <v>66</v>
@@ -7153,7 +7635,7 @@
       </c>
       <c r="N51" s="1"/>
     </row>
-    <row r="52" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C52" s="2" t="s">
         <v>77</v>
       </c>
@@ -7189,7 +7671,7 @@
       </c>
       <c r="N52" s="1"/>
     </row>
-    <row r="53" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C53" s="2" t="s">
         <v>51</v>
       </c>
@@ -7225,7 +7707,7 @@
       </c>
       <c r="N53" s="1"/>
     </row>
-    <row r="54" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C54" s="2" t="s">
         <v>97</v>
       </c>
@@ -7233,359 +7715,739 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="55" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C55" s="3"/>
       <c r="D55" s="63"/>
     </row>
-    <row r="56" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C56" s="3"/>
-      <c r="D56" s="63"/>
-    </row>
-    <row r="57" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C57" s="3"/>
-      <c r="D57" s="63"/>
-    </row>
-    <row r="58" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C58" s="3"/>
-      <c r="D58" s="63"/>
-    </row>
-    <row r="59" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C59" s="3"/>
-      <c r="D59" s="63"/>
-    </row>
-    <row r="60" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C60" s="3"/>
-      <c r="D60" s="63"/>
-    </row>
-    <row r="61" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B61" s="15" t="s">
+    <row r="56" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B56" s="15" t="s">
         <v>89</v>
       </c>
-      <c r="C61" s="16"/>
-      <c r="D61" s="16"/>
-      <c r="E61" s="46"/>
-      <c r="F61" s="17"/>
-      <c r="G61" s="17"/>
-      <c r="H61" s="17"/>
-      <c r="I61" s="17"/>
-      <c r="J61" s="17"/>
-      <c r="K61" s="17"/>
-      <c r="L61" s="17"/>
-      <c r="M61" s="17"/>
-      <c r="N61" s="17"/>
-    </row>
-    <row r="62" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B62" s="3" t="s">
+      <c r="C56" s="16"/>
+      <c r="D56" s="16"/>
+      <c r="E56" s="46"/>
+      <c r="F56" s="17"/>
+      <c r="G56" s="17"/>
+      <c r="H56" s="17"/>
+      <c r="I56" s="17"/>
+      <c r="J56" s="17"/>
+      <c r="K56" s="17"/>
+      <c r="L56" s="17"/>
+      <c r="M56" s="17"/>
+      <c r="N56" s="17"/>
+    </row>
+    <row r="57" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B57" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C62" s="2" t="s">
+      <c r="C57" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="D62" s="44">
+      <c r="D57" s="44">
         <v>0.13</v>
       </c>
-      <c r="E62" s="39" t="s">
+      <c r="E57" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="F62" s="57"/>
-      <c r="G62" s="57"/>
-      <c r="H62" s="57"/>
-      <c r="I62" s="57"/>
-      <c r="J62" s="57"/>
-      <c r="K62" s="57"/>
-      <c r="L62" s="57"/>
-      <c r="M62" s="57"/>
+      <c r="F57" s="57">
+        <v>0.50042799999999998</v>
+      </c>
+      <c r="G57" s="57">
+        <v>0.45500000000000002</v>
+      </c>
+      <c r="H57" s="57">
+        <v>0.47365699999999999</v>
+      </c>
+      <c r="I57" s="57">
+        <v>0.45971400000000001</v>
+      </c>
+      <c r="J57" s="57">
+        <v>0.451986</v>
+      </c>
+      <c r="K57" s="57">
+        <v>0.64251599999999998</v>
+      </c>
+      <c r="L57" s="67">
+        <v>0.40168100000000001</v>
+      </c>
+      <c r="M57" s="57">
+        <v>0.54500000000000004</v>
+      </c>
+      <c r="N57" s="1"/>
+    </row>
+    <row r="58" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C58" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D58" s="55" t="s">
+        <v>104</v>
+      </c>
+      <c r="E58" s="39" t="s">
+        <v>1</v>
+      </c>
+      <c r="F58" s="57">
+        <v>0.47820200000000002</v>
+      </c>
+      <c r="G58" s="67">
+        <v>0.56499999999999995</v>
+      </c>
+      <c r="H58" s="57">
+        <v>0.391982</v>
+      </c>
+      <c r="I58" s="57">
+        <v>0.404644</v>
+      </c>
+      <c r="J58" s="57">
+        <v>0.42641499999999999</v>
+      </c>
+      <c r="K58" s="57">
+        <v>1.8696000000000001E-2</v>
+      </c>
+      <c r="L58" s="57">
+        <v>0.97394999999999998</v>
+      </c>
+      <c r="M58" s="57">
+        <v>0.435</v>
+      </c>
+      <c r="N58" s="1"/>
+    </row>
+    <row r="59" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C59" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D59" s="49">
+        <v>0.05</v>
+      </c>
+      <c r="E59" s="39" t="s">
+        <v>2</v>
+      </c>
+      <c r="F59" s="57">
+        <v>0.49519299999999999</v>
+      </c>
+      <c r="G59" s="57">
+        <v>0.46</v>
+      </c>
+      <c r="H59" s="67">
+        <v>0.48143799999999998</v>
+      </c>
+      <c r="I59" s="67">
+        <v>0.47306300000000001</v>
+      </c>
+      <c r="J59" s="67">
+        <v>0.46745900000000001</v>
+      </c>
+      <c r="K59" s="57">
+        <v>0.55843600000000004</v>
+      </c>
+      <c r="L59" s="57">
+        <v>0.51603200000000005</v>
+      </c>
+      <c r="M59" s="57">
+        <v>0.54</v>
+      </c>
+      <c r="N59" s="1"/>
+    </row>
+    <row r="60" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C60" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D60" s="63">
+        <v>1800</v>
+      </c>
+      <c r="E60" s="35" t="s">
+        <v>3</v>
+      </c>
+      <c r="F60" s="9">
+        <v>0.63498600000000005</v>
+      </c>
+      <c r="G60" s="57">
+        <v>0.58499999999999996</v>
+      </c>
+      <c r="H60" s="57">
+        <v>0.46704200000000001</v>
+      </c>
+      <c r="I60" s="57">
+        <v>0.45617099999999999</v>
+      </c>
+      <c r="J60" s="71">
+        <v>0.46635399999999999</v>
+      </c>
+      <c r="K60" s="9">
+        <v>9.0910000000000001E-3</v>
+      </c>
+      <c r="L60" s="56">
+        <v>0.92254000000000003</v>
+      </c>
+      <c r="M60" s="9">
+        <v>0.41499999999999998</v>
+      </c>
+      <c r="N60" s="42" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="61" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C61" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D61" s="63">
+        <v>1000</v>
+      </c>
+      <c r="E61" s="35"/>
+      <c r="J61" s="7"/>
+      <c r="L61" s="7"/>
+      <c r="M61" s="7"/>
+      <c r="N61" s="1"/>
+    </row>
+    <row r="62" spans="1:14" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D62" s="63"/>
+      <c r="E62" s="35"/>
+      <c r="J62" s="7"/>
+      <c r="L62" s="7"/>
+      <c r="M62" s="7"/>
       <c r="N62" s="1"/>
     </row>
-    <row r="63" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C63" s="2" t="s">
+    <row r="63" spans="1:14" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="70" t="s">
+        <v>138</v>
+      </c>
+      <c r="B63" s="15" t="s">
+        <v>136</v>
+      </c>
+      <c r="C63" s="16"/>
+      <c r="D63" s="16"/>
+      <c r="E63" s="46"/>
+      <c r="F63" s="17"/>
+      <c r="G63" s="17"/>
+      <c r="H63" s="17"/>
+      <c r="I63" s="17"/>
+      <c r="J63" s="17"/>
+      <c r="K63" s="17"/>
+      <c r="L63" s="17"/>
+      <c r="M63" s="17"/>
+      <c r="N63" s="17"/>
+    </row>
+    <row r="64" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B64" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D64" s="44">
+        <v>0.13</v>
+      </c>
+      <c r="E64" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="F64" s="57">
+        <v>0.52957200000000004</v>
+      </c>
+      <c r="G64" s="57">
+        <v>0.47</v>
+      </c>
+      <c r="H64" s="57">
+        <v>0.47777999999999998</v>
+      </c>
+      <c r="I64" s="57">
+        <v>0.45651799999999998</v>
+      </c>
+      <c r="J64" s="57">
+        <v>0.44710100000000003</v>
+      </c>
+      <c r="K64" s="57">
+        <v>0.701824</v>
+      </c>
+      <c r="L64" s="57">
+        <v>0.26685300000000001</v>
+      </c>
+      <c r="M64" s="57">
+        <v>0.53</v>
+      </c>
+      <c r="N64" s="1"/>
+    </row>
+    <row r="65" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C65" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="D63" s="55" t="s">
+      <c r="D65" s="55" t="s">
         <v>104</v>
       </c>
-      <c r="E63" s="39" t="s">
+      <c r="E65" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="F63" s="57"/>
-      <c r="G63" s="57"/>
-      <c r="H63" s="57"/>
-      <c r="I63" s="57"/>
-      <c r="J63" s="57"/>
-      <c r="K63" s="57"/>
-      <c r="L63" s="57"/>
-      <c r="M63" s="57"/>
-      <c r="N63" s="1"/>
-    </row>
-    <row r="64" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C64" s="2" t="s">
+      <c r="F65" s="57">
+        <v>0.423095</v>
+      </c>
+      <c r="G65" s="57">
+        <v>0.63</v>
+      </c>
+      <c r="H65" s="57">
+        <v>0.45200699999999999</v>
+      </c>
+      <c r="I65" s="57">
+        <v>0.47840700000000003</v>
+      </c>
+      <c r="J65" s="57">
+        <v>0.50442200000000004</v>
+      </c>
+      <c r="K65" s="57">
+        <v>2.9266E-2</v>
+      </c>
+      <c r="L65" s="57">
+        <v>1</v>
+      </c>
+      <c r="M65" s="57">
+        <v>0.37</v>
+      </c>
+      <c r="N65" s="1"/>
+    </row>
+    <row r="66" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C66" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="D64" s="49">
+      <c r="D66" s="49">
         <v>0.05</v>
       </c>
-      <c r="E64" s="39" t="s">
+      <c r="E66" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="F64" s="57"/>
-      <c r="G64" s="57"/>
-      <c r="H64" s="57"/>
-      <c r="I64" s="57"/>
-      <c r="J64" s="57"/>
-      <c r="K64" s="57"/>
-      <c r="L64" s="57"/>
-      <c r="M64" s="57"/>
-      <c r="N64" s="1"/>
-    </row>
-    <row r="65" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C65" s="3" t="s">
+      <c r="F66" s="57">
+        <v>0.55037899999999995</v>
+      </c>
+      <c r="G66" s="57">
+        <v>0.51</v>
+      </c>
+      <c r="H66" s="57">
+        <v>0.53003299999999998</v>
+      </c>
+      <c r="I66" s="57">
+        <v>0.51857900000000001</v>
+      </c>
+      <c r="J66" s="57">
+        <v>0.51167200000000002</v>
+      </c>
+      <c r="K66" s="57">
+        <v>0.569886</v>
+      </c>
+      <c r="L66" s="57">
+        <v>0.37756699999999999</v>
+      </c>
+      <c r="M66" s="57">
+        <v>0.49</v>
+      </c>
+      <c r="N66" s="1"/>
+    </row>
+    <row r="67" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C67" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="D65" s="63"/>
-      <c r="E65" s="35" t="s">
+      <c r="D67" s="66">
+        <v>2000</v>
+      </c>
+      <c r="E67" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="F65" s="58"/>
-      <c r="G65" s="58"/>
-      <c r="H65" s="58"/>
-      <c r="I65" s="58"/>
-      <c r="J65" s="58"/>
-      <c r="K65" s="58"/>
-      <c r="L65" s="58"/>
-      <c r="M65" s="58"/>
-      <c r="N65" s="1"/>
-    </row>
-    <row r="66" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C66" s="3" t="s">
+      <c r="F67" s="9">
+        <v>0.82070100000000001</v>
+      </c>
+      <c r="G67" s="9">
+        <v>0.69</v>
+      </c>
+      <c r="H67" s="9">
+        <v>0.73819199999999996</v>
+      </c>
+      <c r="I67" s="9">
+        <v>0.69941799999999998</v>
+      </c>
+      <c r="J67" s="9">
+        <v>0.67926699999999995</v>
+      </c>
+      <c r="K67" s="9">
+        <v>0.50468100000000005</v>
+      </c>
+      <c r="L67" s="9">
+        <v>1.3332999999999999E-2</v>
+      </c>
+      <c r="M67" s="9">
+        <v>0.31</v>
+      </c>
+      <c r="N67" s="69" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="68" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C68" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="D66" s="63"/>
-      <c r="E66" s="35"/>
-      <c r="J66" s="7"/>
-      <c r="L66" s="7"/>
-      <c r="M66" s="7"/>
-      <c r="N66" s="1"/>
-    </row>
-    <row r="67" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B67" s="15" t="s">
+      <c r="D68" s="66">
+        <v>1500</v>
+      </c>
+      <c r="E68" s="35"/>
+      <c r="J68" s="7"/>
+      <c r="L68" s="7"/>
+      <c r="M68" s="7"/>
+      <c r="N68" s="1"/>
+    </row>
+    <row r="69" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D69" s="63"/>
+      <c r="E69" s="35"/>
+      <c r="J69" s="7"/>
+      <c r="L69" s="7"/>
+      <c r="M69" s="7"/>
+      <c r="N69" s="1"/>
+    </row>
+    <row r="70" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B70" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="C67" s="16"/>
-      <c r="D67" s="16"/>
-      <c r="E67" s="46"/>
-      <c r="F67" s="17"/>
-      <c r="G67" s="17"/>
-      <c r="H67" s="17"/>
-      <c r="I67" s="17"/>
-      <c r="J67" s="17"/>
-      <c r="K67" s="17"/>
-      <c r="L67" s="17"/>
-      <c r="M67" s="17"/>
-      <c r="N67" s="17"/>
-    </row>
-    <row r="68" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B68" s="3" t="s">
+      <c r="C70" s="16"/>
+      <c r="D70" s="16"/>
+      <c r="E70" s="46"/>
+      <c r="F70" s="17"/>
+      <c r="G70" s="17"/>
+      <c r="H70" s="17"/>
+      <c r="I70" s="17"/>
+      <c r="J70" s="17"/>
+      <c r="K70" s="17"/>
+      <c r="L70" s="17"/>
+      <c r="M70" s="17"/>
+      <c r="N70" s="17"/>
+    </row>
+    <row r="71" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B71" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C68" s="2" t="s">
+      <c r="C71" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="D68" s="44">
+      <c r="D71" s="44">
         <v>0.13</v>
       </c>
-      <c r="E68" s="39" t="s">
+      <c r="E71" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="F68" s="57"/>
-      <c r="G68" s="57"/>
-      <c r="H68" s="57"/>
-      <c r="I68" s="57"/>
-      <c r="J68" s="57"/>
-      <c r="K68" s="57"/>
-      <c r="L68" s="57"/>
-      <c r="M68" s="57"/>
-      <c r="N68" s="1"/>
-    </row>
-    <row r="69" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C69" s="2" t="s">
+      <c r="F71" s="67">
+        <v>0.55489699999999997</v>
+      </c>
+      <c r="G71" s="57">
+        <v>0.505</v>
+      </c>
+      <c r="H71" s="57">
+        <v>0.469088</v>
+      </c>
+      <c r="I71" s="57">
+        <v>0.44793699999999997</v>
+      </c>
+      <c r="J71" s="57">
+        <v>0.44409300000000002</v>
+      </c>
+      <c r="K71" s="57">
+        <v>0.81087200000000004</v>
+      </c>
+      <c r="L71" s="57">
+        <v>0.142953</v>
+      </c>
+      <c r="M71" s="57">
+        <v>0.495</v>
+      </c>
+      <c r="N71" s="1"/>
+    </row>
+    <row r="72" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C72" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="D69" s="55" t="s">
+      <c r="D72" s="55" t="s">
         <v>105</v>
       </c>
-      <c r="E69" s="39" t="s">
+      <c r="E72" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="F69" s="57"/>
-      <c r="G69" s="57"/>
-      <c r="H69" s="57"/>
-      <c r="I69" s="57"/>
-      <c r="J69" s="57"/>
-      <c r="K69" s="57"/>
-      <c r="L69" s="57"/>
-      <c r="M69" s="57"/>
-      <c r="N69" s="1"/>
-    </row>
-    <row r="70" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C70" s="2" t="s">
+      <c r="F72" s="57">
+        <v>0.35937200000000002</v>
+      </c>
+      <c r="G72" s="57">
+        <v>0.39</v>
+      </c>
+      <c r="H72" s="57">
+        <v>0.23521600000000001</v>
+      </c>
+      <c r="I72" s="57">
+        <v>0.24043400000000001</v>
+      </c>
+      <c r="J72" s="57">
+        <v>0.25619599999999998</v>
+      </c>
+      <c r="K72" s="57">
+        <v>0.98366699999999996</v>
+      </c>
+      <c r="L72" s="67">
+        <v>9.8863999999999994E-2</v>
+      </c>
+      <c r="M72" s="57">
+        <v>0.61</v>
+      </c>
+      <c r="N72" s="1"/>
+    </row>
+    <row r="73" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C73" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="D70" s="49">
+      <c r="D73" s="49">
         <v>0.1</v>
       </c>
-      <c r="E70" s="39" t="s">
+      <c r="E73" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="F70" s="57"/>
-      <c r="G70" s="57"/>
-      <c r="H70" s="57"/>
-      <c r="I70" s="57"/>
-      <c r="J70" s="57"/>
-      <c r="K70" s="57"/>
-      <c r="L70" s="57"/>
-      <c r="M70" s="57"/>
-      <c r="N70" s="1"/>
-    </row>
-    <row r="71" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C71" s="3" t="s">
+      <c r="F73" s="57">
+        <v>0.55212000000000006</v>
+      </c>
+      <c r="G73" s="57">
+        <v>0.495</v>
+      </c>
+      <c r="H73" s="67">
+        <v>0.52401500000000001</v>
+      </c>
+      <c r="I73" s="67">
+        <v>0.50854299999999997</v>
+      </c>
+      <c r="J73" s="67">
+        <v>0.49918299999999999</v>
+      </c>
+      <c r="K73" s="57">
+        <v>0.57175699999999996</v>
+      </c>
+      <c r="L73" s="57">
+        <v>0.38815699999999997</v>
+      </c>
+      <c r="M73" s="57">
+        <v>0.505</v>
+      </c>
+      <c r="N73" s="1"/>
+    </row>
+    <row r="74" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C74" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="D71" s="63"/>
-      <c r="E71" s="35" t="s">
+      <c r="D74" s="63">
+        <v>2500</v>
+      </c>
+      <c r="E74" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="F71" s="58"/>
-      <c r="G71" s="58"/>
-      <c r="H71" s="58"/>
-      <c r="I71" s="58"/>
-      <c r="J71" s="58"/>
-      <c r="K71" s="58"/>
-      <c r="L71" s="58"/>
-      <c r="M71" s="58"/>
-      <c r="N71" s="1"/>
-    </row>
-    <row r="72" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C72" s="3" t="s">
+      <c r="F74" s="57">
+        <v>0.40412500000000001</v>
+      </c>
+      <c r="G74" s="9">
+        <v>0.63500000000000001</v>
+      </c>
+      <c r="H74" s="57">
+        <v>0.43570199999999998</v>
+      </c>
+      <c r="I74" s="57">
+        <v>0.46478700000000001</v>
+      </c>
+      <c r="J74" s="71">
+        <v>0.49365399999999998</v>
+      </c>
+      <c r="K74" s="9">
+        <v>0</v>
+      </c>
+      <c r="L74" s="56">
+        <v>1</v>
+      </c>
+      <c r="M74" s="9">
+        <v>0.36499999999999999</v>
+      </c>
+      <c r="N74" s="1"/>
+    </row>
+    <row r="75" spans="1:14" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C75" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="D72" s="63"/>
-      <c r="N72" s="1"/>
-    </row>
-    <row r="73" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B73" s="15" t="s">
-        <v>112</v>
-      </c>
-      <c r="C73" s="16"/>
-      <c r="D73" s="16"/>
-      <c r="E73" s="46"/>
-      <c r="F73" s="17"/>
-      <c r="G73" s="17"/>
-      <c r="H73" s="17"/>
-      <c r="I73" s="17"/>
-      <c r="J73" s="17"/>
-      <c r="K73" s="17"/>
-      <c r="L73" s="17"/>
-      <c r="M73" s="17"/>
-      <c r="N73" s="17"/>
-    </row>
-    <row r="74" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B74" s="3" t="s">
+      <c r="D75" s="63">
+        <v>2000</v>
+      </c>
+      <c r="N75" s="1"/>
+    </row>
+    <row r="76" spans="1:14" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A76" s="70" t="s">
+        <v>138</v>
+      </c>
+      <c r="B76" s="15" t="s">
+        <v>140</v>
+      </c>
+      <c r="C76" s="16"/>
+      <c r="D76" s="16"/>
+      <c r="E76" s="46"/>
+      <c r="F76" s="17"/>
+      <c r="G76" s="17"/>
+      <c r="H76" s="17"/>
+      <c r="I76" s="17"/>
+      <c r="J76" s="17"/>
+      <c r="K76" s="17"/>
+      <c r="L76" s="17"/>
+      <c r="M76" s="17"/>
+      <c r="N76" s="17"/>
+    </row>
+    <row r="77" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>141</v>
+      </c>
+      <c r="B77" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C74" s="2" t="s">
+      <c r="C77" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="D74" s="44">
+      <c r="D77" s="44">
         <v>0.13</v>
       </c>
-      <c r="E74" s="39" t="s">
+      <c r="E77" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="F74" s="57"/>
-      <c r="G74" s="57"/>
-      <c r="H74" s="57"/>
-      <c r="I74" s="57"/>
-      <c r="J74" s="57"/>
-      <c r="K74" s="57"/>
-      <c r="L74" s="57"/>
-      <c r="M74" s="57"/>
-      <c r="N74" s="1"/>
-    </row>
-    <row r="75" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C75" s="2" t="s">
+      <c r="F77" s="57">
+        <v>0.48685200000000001</v>
+      </c>
+      <c r="G77" s="57">
+        <v>0.45500000000000002</v>
+      </c>
+      <c r="H77" s="57">
+        <v>0.47313100000000002</v>
+      </c>
+      <c r="I77" s="57">
+        <v>0.465032</v>
+      </c>
+      <c r="J77" s="57">
+        <v>0.45982600000000001</v>
+      </c>
+      <c r="K77" s="57">
+        <v>0.53969299999999998</v>
+      </c>
+      <c r="L77" s="57">
+        <v>0.55131200000000002</v>
+      </c>
+      <c r="M77" s="57">
+        <v>0.54500000000000004</v>
+      </c>
+      <c r="N77" s="1"/>
+    </row>
+    <row r="78" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C78" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="D75" s="55" t="s">
+      <c r="D78" s="55" t="s">
         <v>105</v>
       </c>
-      <c r="E75" s="39" t="s">
+      <c r="E78" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="F75" s="57"/>
-      <c r="G75" s="57"/>
-      <c r="H75" s="57"/>
-      <c r="I75" s="57"/>
-      <c r="J75" s="57"/>
-      <c r="K75" s="57"/>
-      <c r="L75" s="57"/>
-      <c r="M75" s="57"/>
-      <c r="N75" s="1"/>
-    </row>
-    <row r="76" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C76" s="2" t="s">
+      <c r="F78" s="57">
+        <v>0.40894200000000003</v>
+      </c>
+      <c r="G78" s="57">
+        <v>0.63</v>
+      </c>
+      <c r="H78" s="57">
+        <v>0.43956400000000001</v>
+      </c>
+      <c r="I78" s="57">
+        <v>0.46764899999999998</v>
+      </c>
+      <c r="J78" s="57">
+        <v>0.49541499999999999</v>
+      </c>
+      <c r="K78" s="67">
+        <v>1.5476E-2</v>
+      </c>
+      <c r="L78" s="57">
+        <v>1</v>
+      </c>
+      <c r="M78" s="57">
+        <v>0.37</v>
+      </c>
+      <c r="N78" s="1"/>
+    </row>
+    <row r="79" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C79" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="D76" s="49">
+      <c r="D79" s="49">
         <v>0.1</v>
       </c>
-      <c r="E76" s="39" t="s">
+      <c r="E79" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="F76" s="57"/>
-      <c r="G76" s="57"/>
-      <c r="H76" s="57"/>
-      <c r="I76" s="57"/>
-      <c r="J76" s="57"/>
-      <c r="K76" s="57"/>
-      <c r="L76" s="57"/>
-      <c r="M76" s="57"/>
-      <c r="N76" s="1"/>
-    </row>
-    <row r="77" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C77" s="3" t="s">
+      <c r="F79" s="57">
+        <v>0.52954400000000001</v>
+      </c>
+      <c r="G79" s="57">
+        <v>0.48499999999999999</v>
+      </c>
+      <c r="H79" s="57">
+        <v>0.51397499999999996</v>
+      </c>
+      <c r="I79" s="57">
+        <v>0.50402000000000002</v>
+      </c>
+      <c r="J79" s="57">
+        <v>0.497029</v>
+      </c>
+      <c r="K79" s="57">
+        <v>0.50992099999999996</v>
+      </c>
+      <c r="L79" s="57">
+        <v>0.53269200000000005</v>
+      </c>
+      <c r="M79" s="57">
+        <v>0.51500000000000001</v>
+      </c>
+      <c r="N79" s="1"/>
+    </row>
+    <row r="80" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C80" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="D77" s="63"/>
-      <c r="E77" s="35" t="s">
+      <c r="D80" s="63">
+        <v>1000</v>
+      </c>
+      <c r="E80" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="F77" s="58"/>
-      <c r="G77" s="58"/>
-      <c r="H77" s="58"/>
-      <c r="I77" s="58"/>
-      <c r="J77" s="58"/>
-      <c r="K77" s="58"/>
-      <c r="L77" s="58"/>
-      <c r="M77" s="58"/>
-      <c r="N77" s="1"/>
-    </row>
-    <row r="78" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C78" s="3" t="s">
+      <c r="F80" s="9">
+        <v>0.73575000000000002</v>
+      </c>
+      <c r="G80" s="9">
+        <v>0.72499999999999998</v>
+      </c>
+      <c r="H80" s="9">
+        <v>0.70614500000000002</v>
+      </c>
+      <c r="I80" s="9">
+        <v>0.696523</v>
+      </c>
+      <c r="J80" s="9">
+        <v>0.69491099999999995</v>
+      </c>
+      <c r="K80" s="71">
+        <v>7.0999000000000007E-2</v>
+      </c>
+      <c r="L80" s="9">
+        <v>0.62804700000000002</v>
+      </c>
+      <c r="M80" s="9">
+        <v>0.27500000000000002</v>
+      </c>
+      <c r="N80" s="69" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="81" spans="3:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C81" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="D78" s="63"/>
-      <c r="N78" s="1"/>
-    </row>
-    <row r="79" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="C79" s="6"/>
-      <c r="N79" s="1"/>
-    </row>
-    <row r="80" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="C80" s="6"/>
-      <c r="N80" s="1"/>
-    </row>
-    <row r="81" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C81" s="6"/>
+      <c r="D81" s="63">
+        <v>1000</v>
+      </c>
       <c r="N81" s="1"/>
     </row>
     <row r="82" spans="3:14" x14ac:dyDescent="0.25">
@@ -7725,60 +8587,73 @@
       <c r="N115" s="1"/>
     </row>
     <row r="116" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="C116" s="6"/>
       <c r="N116" s="1"/>
     </row>
     <row r="117" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="C117" s="6"/>
       <c r="N117" s="1"/>
     </row>
     <row r="118" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="E118" s="35"/>
+      <c r="C118" s="6"/>
       <c r="N118" s="1"/>
     </row>
     <row r="119" spans="2:14" x14ac:dyDescent="0.25">
       <c r="N119" s="1"/>
     </row>
     <row r="120" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B120" s="22" t="s">
+      <c r="N120" s="1"/>
+    </row>
+    <row r="121" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="E121" s="35"/>
+      <c r="N121" s="1"/>
+    </row>
+    <row r="122" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="N122" s="1"/>
+    </row>
+    <row r="123" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B123" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="C120" s="23"/>
-      <c r="D120" s="23"/>
-      <c r="E120" s="47"/>
-      <c r="F120" s="24"/>
-      <c r="G120" s="24"/>
-      <c r="H120" s="24"/>
-      <c r="I120" s="24"/>
-      <c r="J120" s="24"/>
-      <c r="K120" s="24"/>
-      <c r="L120" s="25"/>
-      <c r="M120" s="43"/>
-    </row>
-    <row r="121" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B121"/>
-      <c r="C121"/>
-      <c r="D121"/>
-      <c r="E121" s="3"/>
-      <c r="F121"/>
-      <c r="G121"/>
-      <c r="H121"/>
-      <c r="I121"/>
-      <c r="J121"/>
-      <c r="K121"/>
-      <c r="L121"/>
-      <c r="M121"/>
-    </row>
-    <row r="136" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P136" s="3"/>
-      <c r="Q136"/>
-      <c r="R136"/>
-    </row>
-    <row r="137" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="Q137"/>
-      <c r="R137"/>
+      <c r="C123" s="23"/>
+      <c r="D123" s="23"/>
+      <c r="E123" s="47"/>
+      <c r="F123" s="24"/>
+      <c r="G123" s="24"/>
+      <c r="H123" s="24"/>
+      <c r="I123" s="24"/>
+      <c r="J123" s="24"/>
+      <c r="K123" s="24"/>
+      <c r="L123" s="25"/>
+      <c r="M123" s="43"/>
+    </row>
+    <row r="124" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B124"/>
+      <c r="C124"/>
+      <c r="D124"/>
+      <c r="E124" s="3"/>
+      <c r="F124"/>
+      <c r="G124"/>
+      <c r="H124"/>
+      <c r="I124"/>
+      <c r="J124"/>
+      <c r="K124"/>
+      <c r="L124"/>
+      <c r="M124"/>
+    </row>
+    <row r="139" spans="16:18" x14ac:dyDescent="0.25">
+      <c r="P139" s="3"/>
+      <c r="Q139"/>
+      <c r="R139"/>
+    </row>
+    <row r="140" spans="16:18" x14ac:dyDescent="0.25">
+      <c r="Q140"/>
+      <c r="R140"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -7788,7 +8663,7 @@
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D5" sqref="D5"/>
+      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8042,7 +8917,7 @@
     </row>
     <row r="21" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C21" s="59" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="J21" s="3"/>
       <c r="L21" s="3"/>
@@ -8050,7 +8925,7 @@
     </row>
     <row r="22" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C22" s="59" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="J22" s="3"/>
       <c r="L22" s="3"/>
@@ -8188,16 +9063,16 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="60"/>
       <c r="B2" s="60" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C2" s="64" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D2" s="60">
         <v>2022</v>
@@ -8207,10 +9082,10 @@
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="60"/>
       <c r="B3" s="60" t="s">
+        <v>123</v>
+      </c>
+      <c r="C3" s="64" t="s">
         <v>124</v>
-      </c>
-      <c r="C3" s="64" t="s">
-        <v>125</v>
       </c>
       <c r="D3" s="60">
         <v>2007</v>
@@ -8220,33 +9095,33 @@
     <row r="4" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A4" s="60"/>
       <c r="B4" s="60" t="s">
+        <v>128</v>
+      </c>
+      <c r="C4" s="64" t="s">
         <v>129</v>
-      </c>
-      <c r="C4" s="64" t="s">
-        <v>130</v>
       </c>
       <c r="D4" s="60">
         <v>2011</v>
       </c>
       <c r="E4" s="65" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="5" spans="1:5" s="60" customFormat="1" ht="165" x14ac:dyDescent="0.25">
       <c r="A5" s="60" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B5" s="60" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C5" s="64" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D5" s="60">
         <v>2020</v>
       </c>
       <c r="E5" s="65" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
V.8.9 Added title and sub-title (file names) to plots
</commit_message>
<xml_diff>
--- a/analysis/Analysis_Experiments_V5_13-May-2023.xlsx
+++ b/analysis/Analysis_Experiments_V5_13-May-2023.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Rajesh\ResearchLab\RL_for_PdM\REINFORCE_Tool_Replace_Policy\analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4248E27B-2409-46E8-AE46-71CAACF456AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B66A98D-9162-4131-991E-35F1243621B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="506" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="506" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Simulated Env. Expts." sheetId="9" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="538" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="147">
   <si>
     <t>A2C</t>
   </si>
@@ -825,6 +825,21 @@
   </si>
   <si>
     <t>Lower ep./term</t>
+  </si>
+  <si>
+    <t>Dasic_NoNoise_3.0__test_results_13-May-2023</t>
+  </si>
+  <si>
+    <t>Dasic_LowNBD_3.0__test_results_13-May-2023-07</t>
+  </si>
+  <si>
+    <t>Dasic_HighNBD_3.0__test_results_13-May-2023-45</t>
+  </si>
+  <si>
+    <t>PHM_C01_HighNBD_0.12_100.0_0.1_test_results_13-May-2023-03</t>
+  </si>
+  <si>
+    <t>PHM_C01_LowNBD_0.12_1000.0_0.05_test_results_13-May-2023-50</t>
   </si>
 </sst>
 </file>
@@ -3147,7 +3162,7 @@
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N26" sqref="N26"/>
+      <selection pane="bottomLeft" activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3237,7 +3252,9 @@
       <c r="H5" s="17"/>
       <c r="I5" s="17"/>
       <c r="J5" s="17"/>
-      <c r="K5" s="17"/>
+      <c r="K5" s="17" t="s">
+        <v>142</v>
+      </c>
       <c r="L5" s="17"/>
       <c r="M5" s="17"/>
       <c r="N5" s="17"/>
@@ -3421,7 +3438,9 @@
       <c r="H11" s="17"/>
       <c r="I11" s="17"/>
       <c r="J11" s="17"/>
-      <c r="K11" s="17"/>
+      <c r="K11" s="17" t="s">
+        <v>143</v>
+      </c>
       <c r="L11" s="17"/>
       <c r="M11" s="17"/>
       <c r="N11" s="17"/>
@@ -3619,7 +3638,9 @@
       <c r="H17" s="17"/>
       <c r="I17" s="17"/>
       <c r="J17" s="17"/>
-      <c r="K17" s="17"/>
+      <c r="K17" s="17" t="s">
+        <v>144</v>
+      </c>
       <c r="L17" s="17"/>
       <c r="M17" s="17"/>
       <c r="N17" s="17"/>
@@ -4047,9 +4068,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D002316C-426C-49E1-8B50-2FDC1BA0BFFE}">
   <dimension ref="A2:W87"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="S12" sqref="S12"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4375,7 +4396,9 @@
       <c r="H11" s="17"/>
       <c r="I11" s="17"/>
       <c r="J11" s="17"/>
-      <c r="K11" s="17"/>
+      <c r="K11" s="17" t="s">
+        <v>146</v>
+      </c>
       <c r="L11" s="17"/>
       <c r="M11" s="17"/>
       <c r="N11" s="17"/>
@@ -4583,7 +4606,9 @@
       <c r="H17" s="17"/>
       <c r="I17" s="17"/>
       <c r="J17" s="17"/>
-      <c r="K17" s="17"/>
+      <c r="K17" s="17" t="s">
+        <v>145</v>
+      </c>
       <c r="L17" s="17"/>
       <c r="M17" s="17"/>
       <c r="N17" s="17"/>
@@ -6202,9 +6227,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE699FEF-4516-4E3F-8EE7-4192FF715912}">
   <dimension ref="A2:W140"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M21" sqref="M21"/>
+      <selection pane="bottomLeft" activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7014,14 +7039,30 @@
       <c r="E25" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="F25" s="57"/>
-      <c r="G25" s="57"/>
-      <c r="H25" s="57"/>
-      <c r="I25" s="57"/>
-      <c r="J25" s="57"/>
-      <c r="K25" s="57"/>
-      <c r="L25" s="57"/>
-      <c r="M25" s="57"/>
+      <c r="F25" s="57">
+        <v>0.47562399999999999</v>
+      </c>
+      <c r="G25" s="57">
+        <v>0.505</v>
+      </c>
+      <c r="H25" s="57">
+        <v>0.45020500000000002</v>
+      </c>
+      <c r="I25" s="57">
+        <v>0.44553900000000002</v>
+      </c>
+      <c r="J25" s="57">
+        <v>0.44889000000000001</v>
+      </c>
+      <c r="K25" s="57">
+        <v>0.82901899999999995</v>
+      </c>
+      <c r="L25" s="67">
+        <v>0.19778000000000001</v>
+      </c>
+      <c r="M25" s="57">
+        <v>0.495</v>
+      </c>
       <c r="Q25"/>
       <c r="R25"/>
     </row>
@@ -7036,14 +7077,30 @@
       <c r="E26" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="F26" s="57"/>
-      <c r="G26" s="57"/>
-      <c r="H26" s="57"/>
-      <c r="I26" s="57"/>
-      <c r="J26" s="57"/>
-      <c r="K26" s="57"/>
-      <c r="L26" s="57"/>
-      <c r="M26" s="57"/>
+      <c r="F26" s="57">
+        <v>0.34883900000000001</v>
+      </c>
+      <c r="G26" s="57">
+        <v>0.45</v>
+      </c>
+      <c r="H26" s="57">
+        <v>0.26862599999999998</v>
+      </c>
+      <c r="I26" s="57">
+        <v>0.27943699999999999</v>
+      </c>
+      <c r="J26" s="57">
+        <v>0.29936699999999999</v>
+      </c>
+      <c r="K26" s="57">
+        <v>3.1746000000000003E-2</v>
+      </c>
+      <c r="L26" s="57">
+        <v>0.98138499999999995</v>
+      </c>
+      <c r="M26" s="57">
+        <v>0.55000000000000004</v>
+      </c>
       <c r="Q26"/>
       <c r="R26"/>
     </row>
@@ -7057,14 +7114,30 @@
       <c r="E27" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="F27" s="57"/>
-      <c r="G27" s="57"/>
-      <c r="H27" s="57"/>
-      <c r="I27" s="57"/>
-      <c r="J27" s="57"/>
-      <c r="K27" s="57"/>
-      <c r="L27" s="57"/>
-      <c r="M27" s="57"/>
+      <c r="F27" s="57">
+        <v>0.50987499999999997</v>
+      </c>
+      <c r="G27" s="57">
+        <v>0.505</v>
+      </c>
+      <c r="H27" s="57">
+        <v>0.50178299999999998</v>
+      </c>
+      <c r="I27" s="57">
+        <v>0.49864999999999998</v>
+      </c>
+      <c r="J27" s="57">
+        <v>0.49767800000000001</v>
+      </c>
+      <c r="K27" s="57">
+        <v>0.443463</v>
+      </c>
+      <c r="L27" s="57">
+        <v>0.547342</v>
+      </c>
+      <c r="M27" s="57">
+        <v>0.495</v>
+      </c>
       <c r="Q27"/>
       <c r="R27"/>
     </row>
@@ -7072,18 +7145,36 @@
       <c r="C28" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="D28" s="63"/>
+      <c r="D28" s="63">
+        <v>1200</v>
+      </c>
       <c r="E28" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="F28" s="58"/>
-      <c r="G28" s="58"/>
-      <c r="H28" s="58"/>
-      <c r="I28" s="58"/>
-      <c r="J28" s="58"/>
-      <c r="K28" s="58"/>
-      <c r="L28" s="58"/>
-      <c r="M28" s="58"/>
+      <c r="F28" s="9">
+        <v>0.78775300000000004</v>
+      </c>
+      <c r="G28" s="9">
+        <v>0.64</v>
+      </c>
+      <c r="H28" s="9">
+        <v>0.65794900000000001</v>
+      </c>
+      <c r="I28" s="9">
+        <v>0.61424100000000004</v>
+      </c>
+      <c r="J28" s="9">
+        <v>0.59743100000000005</v>
+      </c>
+      <c r="K28" s="9">
+        <v>9.5239999999999995E-3</v>
+      </c>
+      <c r="L28" s="57">
+        <v>0.67124399999999995</v>
+      </c>
+      <c r="M28" s="9">
+        <v>0.36</v>
+      </c>
       <c r="Q28"/>
       <c r="R28"/>
     </row>
@@ -7091,7 +7182,9 @@
       <c r="C29" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="D29" s="63"/>
+      <c r="D29" s="63">
+        <v>800</v>
+      </c>
       <c r="Q29"/>
       <c r="R29"/>
     </row>

</xml_diff>